<commit_message>
quadro de cargas nao havia sido salvo
</commit_message>
<xml_diff>
--- a/Quadro de cargas - Maquinas.xlsx
+++ b/Quadro de cargas - Maquinas.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\Documents\Giovani\UCS\Instalações Elétricas (2)\UCS_Instalacao_Eletrica_Residencial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\Documents\Giovani\UCS\Instalações Elétricas (2)\UCS_Projeto_Instala-es_Industriais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940FF5C9-8C1A-4EB6-A75A-8D0ABC80ABF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F35E4C9-40A3-473C-B514-0384FAA99946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2475" windowWidth="20640" windowHeight="11760" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quadro de cargas" sheetId="1" r:id="rId1"/>
-    <sheet name="Alimentador" sheetId="5" r:id="rId2"/>
-    <sheet name="Cômodos" sheetId="2" r:id="rId3"/>
-    <sheet name="Parâmetros" sheetId="3" r:id="rId4"/>
-    <sheet name="Cabos" sheetId="4" r:id="rId5"/>
+    <sheet name="Maquinas" sheetId="6" r:id="rId2"/>
+    <sheet name="Alimentador" sheetId="5" r:id="rId3"/>
+    <sheet name="Cômodos" sheetId="2" r:id="rId4"/>
+    <sheet name="Parâmetros" sheetId="3" r:id="rId5"/>
+    <sheet name="Cabos" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Cargas de Iluminação</t>
   </si>
@@ -100,9 +101,6 @@
   </si>
   <si>
     <t>Chuveiro 1</t>
-  </si>
-  <si>
-    <t>Chuveiro 2</t>
   </si>
   <si>
     <t>Cômodo</t>
@@ -143,83 +141,26 @@
     <t>Banheiro 1</t>
   </si>
   <si>
-    <t>Cozinha</t>
-  </si>
-  <si>
     <t>CARGAS DE FORÇA
 (tomadas elétricas)</t>
   </si>
   <si>
-    <t>Área de serviço</t>
-  </si>
-  <si>
     <t>Área</t>
   </si>
   <si>
     <t>Perímetro</t>
   </si>
   <si>
-    <t>Sala</t>
-  </si>
-  <si>
-    <t>Quarto 1</t>
-  </si>
-  <si>
-    <t>Quarto 2</t>
-  </si>
-  <si>
-    <t>Suíte</t>
-  </si>
-  <si>
-    <t>Circulação</t>
-  </si>
-  <si>
-    <t>Varanda Q1</t>
-  </si>
-  <si>
-    <t>Garagem</t>
-  </si>
-  <si>
-    <t>Tomadas</t>
-  </si>
-  <si>
     <t>Tomadas (min)</t>
   </si>
   <si>
     <t>Tensão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banheiro1 </t>
-  </si>
-  <si>
-    <t>Ilumimnação</t>
   </si>
   <si>
     <t>Iluminação
 (min)</t>
   </si>
   <si>
-    <t>Banheiro1</t>
-  </si>
-  <si>
-    <t>Varanda Suíte</t>
-  </si>
-  <si>
-    <t>Banheiro Suíte</t>
-  </si>
-  <si>
-    <t>2x100
-1x600</t>
-  </si>
-  <si>
-    <t>4x100
-6x600</t>
-  </si>
-  <si>
-    <t>1x100
-2x600</t>
-  </si>
-  <si>
     <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://www.guiadaengenharia.com/wp-content/uploads/2019/02/tabelas-completas-5410.pdf</t>
   </si>
   <si>
@@ -232,12 +173,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>Carregador EV</t>
-  </si>
-  <si>
-    <t>Externa</t>
-  </si>
-  <si>
     <t>Potência</t>
   </si>
   <si>
@@ -293,6 +228,93 @@
   </si>
   <si>
     <t>16mm²</t>
+  </si>
+  <si>
+    <t>Máquina</t>
+  </si>
+  <si>
+    <t>Printer YSP10</t>
+  </si>
+  <si>
+    <t>Alimentação</t>
+  </si>
+  <si>
+    <t>Especificações</t>
+  </si>
+  <si>
+    <t>https://global.yamaha-motor.com/business/smt/printer/ysp10/spec/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conveyor </t>
+  </si>
+  <si>
+    <t>https://www.allpoint.com.br/transportador-de-inspecao-e-conexao.html</t>
+  </si>
+  <si>
+    <t>220 VAC / 60Hz / Monofásico 120W</t>
+  </si>
+  <si>
+    <t>Single-phase AC 200 to 230V +/-20V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic pick and place AM100 </t>
+  </si>
+  <si>
+    <t>3-phase AC 200 / 220 V ±10 V, AC 380 / 400 / 420 / 480 V ±20 V 2.0 kVA</t>
+  </si>
+  <si>
+    <t>https://na.panasonic.com/us/factory-equipment-solutions/electronics-assembly-manufacturing-technologies/surface-mount-technology-smt/am100-single-beam-single-head-placement</t>
+  </si>
+  <si>
+    <t>5 linhas, 3 fases 380V 50/60Hz 68kW</t>
+  </si>
+  <si>
+    <t>https://www.allpoint.com.br/forno-de-refusao-point-reflow-12-zonas.html</t>
+  </si>
+  <si>
+    <t>Reflow oven Point reflow 12 zonas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wave solder tnw33-36ex/et </t>
+  </si>
+  <si>
+    <t>AC220V±10% -50/60Hz-3φ 34kVA 95A</t>
+  </si>
+  <si>
+    <t>https://www.tamuracorp.com/products/electronic_chemicals/category/fa_systems/w_solder/tnw.html</t>
+  </si>
+  <si>
+    <t>AOI</t>
+  </si>
+  <si>
+    <t>https://www.vitrox.com/vision-technology-machine-system/optical-inspection-system-aoi-v510i-se-spec.php</t>
+  </si>
+  <si>
+    <t>100-120 V, 16A / 200-240V, 8A Single Phase</t>
+  </si>
+  <si>
+    <t>Bancada de uso geral</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Computador + monitor 21"</t>
+  </si>
+  <si>
+    <t>Hot air station</t>
+  </si>
+  <si>
+    <t>Soldering station</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Iluminação</t>
+  </si>
+  <si>
+    <t>220V - 1980W</t>
   </si>
 </sst>
 </file>
@@ -302,7 +324,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -348,6 +370,20 @@
     <font>
       <u/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -545,11 +581,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -681,89 +718,108 @@
     <xf numFmtId="2" fontId="3" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1175,8 +1231,8 @@
   </sheetPr>
   <dimension ref="A1:X38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X33" sqref="A1:X33"/>
+    <sheetView topLeftCell="B5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T24" sqref="S8:T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1210,21 +1266,21 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="77" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
+      <c r="F1" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
@@ -1240,45 +1296,45 @@
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="77" t="s">
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77" t="s">
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77" t="s">
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="75" t="s">
+      <c r="Q2" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="75" t="s">
+      <c r="R2" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="75" t="s">
+      <c r="S2" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="75" t="s">
+      <c r="T2" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="75" t="s">
+      <c r="U2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="75" t="s">
+      <c r="V2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="75" t="s">
+      <c r="W2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="X2" s="75" t="s">
+      <c r="X2" s="51" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1287,16 +1343,16 @@
         <v>9</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="F3" s="38" t="s">
         <v>10</v>
@@ -1328,15 +1384,15 @@
       <c r="O3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="76"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="52"/>
+      <c r="U3" s="52"/>
+      <c r="V3" s="52"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
     </row>
     <row r="4" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -1346,15 +1402,15 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="19">
         <f>Cômodos!B2</f>
-        <v>5.61</v>
+        <v>0</v>
       </c>
       <c r="E4" s="19">
         <f>Cômodos!C2</f>
-        <v>9.91</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1369,20 +1425,18 @@
       <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="N4" s="1">
-        <v>7400</v>
-      </c>
+      <c r="N4" s="1"/>
       <c r="O4" s="1">
         <f>N4*M4</f>
-        <v>7400</v>
+        <v>0</v>
       </c>
       <c r="P4" s="14">
         <f>O4+L4</f>
-        <v>7400</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="19">
         <f>P4/Parâmetros!$B$1</f>
-        <v>33.636363636363633</v>
+        <v>0</v>
       </c>
       <c r="R4" s="1">
         <f>Parâmetros!$B$2</f>
@@ -1394,7 +1448,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="19">
         <f>Q4/(R4*S4)</f>
-        <v>31.732418524871349</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1">
         <v>6</v>
@@ -1403,27 +1457,17 @@
         <v>32</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>2</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="28">
-        <f>Cômodos!B3</f>
-        <v>5.36</v>
-      </c>
-      <c r="E5" s="28">
-        <f>Cômodos!C3</f>
-        <v>9.76</v>
-      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -1437,20 +1481,18 @@
       <c r="M5" s="29">
         <v>1</v>
       </c>
-      <c r="N5" s="29">
-        <v>7400</v>
-      </c>
+      <c r="N5" s="29"/>
       <c r="O5" s="29">
         <f t="shared" ref="O5:O6" si="1">N5*M5</f>
-        <v>7400</v>
+        <v>0</v>
       </c>
       <c r="P5" s="27">
         <f t="shared" ref="P5:P7" si="2">O5+L5</f>
-        <v>7400</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="28">
         <f>P5/Parâmetros!$B$1</f>
-        <v>33.636363636363633</v>
+        <v>0</v>
       </c>
       <c r="R5" s="29">
         <f>Parâmetros!$B$2</f>
@@ -1462,7 +1504,7 @@
       <c r="T5" s="29"/>
       <c r="U5" s="28">
         <f t="shared" ref="U5:U7" si="3">Q5/(R5*S5)</f>
-        <v>31.732418524871349</v>
+        <v>0</v>
       </c>
       <c r="V5" s="29">
         <v>6</v>
@@ -1471,35 +1513,23 @@
         <v>32</v>
       </c>
       <c r="X5" s="29" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="19">
-        <f>Cômodos!B4</f>
-        <v>11.4</v>
-      </c>
-      <c r="E6" s="19">
-        <f>Cômodos!C4</f>
-        <v>13.7</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="14"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="K6" s="1"/>
       <c r="L6" s="1">
         <f>4*100+6*600</f>
         <v>4000</v>
@@ -1507,20 +1537,18 @@
       <c r="M6" s="1">
         <v>2</v>
       </c>
-      <c r="N6" s="1">
-        <v>1400</v>
-      </c>
+      <c r="N6" s="1"/>
       <c r="O6" s="1">
         <f t="shared" si="1"/>
-        <v>2800</v>
+        <v>0</v>
       </c>
       <c r="P6" s="14">
         <f t="shared" si="2"/>
-        <v>6800</v>
+        <v>4000</v>
       </c>
       <c r="Q6" s="19">
         <f>P6/Parâmetros!$B$1</f>
-        <v>30.90909090909091</v>
+        <v>18.181818181818183</v>
       </c>
       <c r="R6" s="1">
         <f>Parâmetros!$B$2</f>
@@ -1532,7 +1560,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="19">
         <f t="shared" si="3"/>
-        <v>29.159519725557463</v>
+        <v>17.152658662092627</v>
       </c>
       <c r="V6" s="1">
         <v>6</v>
@@ -1541,37 +1569,23 @@
         <v>32</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>4</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="28">
-        <f>Cômodos!B5</f>
-        <v>6</v>
-      </c>
-      <c r="E7" s="28">
-        <f>Cômodos!C5</f>
-        <v>10</v>
-      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
       <c r="H7" s="29"/>
       <c r="I7" s="27"/>
-      <c r="J7" s="29">
-        <v>3</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>47</v>
-      </c>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
       <c r="L7" s="29">
         <f>100+2*600</f>
         <v>1300</v>
@@ -1606,35 +1620,23 @@
         <v>16</v>
       </c>
       <c r="X7" s="29" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62">
+      <c r="A8" s="56">
         <v>5</v>
       </c>
-      <c r="B8" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="19">
-        <f>Cômodos!B2</f>
-        <v>5.61</v>
-      </c>
-      <c r="E8" s="19">
-        <f>Cômodos!C2</f>
-        <v>9.91</v>
-      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="14"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="K8" s="1"/>
       <c r="L8" s="1">
         <f>1*100+2*600</f>
         <v>1300</v>
@@ -1644,11 +1646,11 @@
       <c r="O8" s="1"/>
       <c r="P8" s="53">
         <f>O8+O9+L8+L9+O10+L10</f>
-        <v>2800</v>
+        <v>2600</v>
       </c>
       <c r="Q8" s="59">
         <f>P8/Parâmetros!$B$1</f>
-        <v>12.727272727272727</v>
+        <v>11.818181818181818</v>
       </c>
       <c r="R8" s="53">
         <f>Parâmetros!$B$2</f>
@@ -1660,7 +1662,7 @@
       <c r="T8" s="53"/>
       <c r="U8" s="59">
         <f>Q8/(R8*S8)</f>
-        <v>17.152658662092623</v>
+        <v>15.927468757657437</v>
       </c>
       <c r="V8" s="53">
         <v>2.5</v>
@@ -1669,31 +1671,21 @@
         <v>16</v>
       </c>
       <c r="X8" s="53" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="63"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="54"/>
-      <c r="C9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="19">
-        <f>Cômodos!B3</f>
-        <v>5.36</v>
-      </c>
-      <c r="E9" s="19">
-        <f>Cômodos!C3</f>
-        <v>9.76</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="14"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="K9" s="1"/>
       <c r="L9" s="1">
         <f>1*100+2*600</f>
         <v>1300</v>
@@ -1712,32 +1704,20 @@
       <c r="X9" s="54"/>
     </row>
     <row r="10" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="55"/>
-      <c r="C10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="19">
-        <f>+Cômodos!B10</f>
-        <v>8.5</v>
-      </c>
-      <c r="E10" s="19">
-        <f>+Cômodos!C10</f>
-        <v>13.25</v>
-      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="14"/>
-      <c r="J10" s="1">
-        <v>2</v>
-      </c>
-      <c r="K10" s="1">
-        <v>100</v>
-      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
       <c r="L10" s="1">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1753,153 +1733,113 @@
       <c r="X10" s="55"/>
     </row>
     <row r="11" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="72">
+      <c r="A11" s="65">
         <v>6</v>
       </c>
-      <c r="B11" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="28">
-        <f>Cômodos!B9</f>
-        <v>17</v>
-      </c>
-      <c r="E11" s="28">
-        <f>Cômodos!C9</f>
-        <v>16.899999999999999</v>
-      </c>
+      <c r="B11" s="63"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
-      <c r="J11" s="29">
-        <v>6</v>
-      </c>
-      <c r="K11" s="29">
-        <v>100</v>
-      </c>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
       <c r="L11" s="29">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M11" s="29"/>
       <c r="N11" s="29"/>
       <c r="O11" s="29"/>
-      <c r="P11" s="56">
+      <c r="P11" s="63">
         <f>O11+O12+L12+L11</f>
-        <v>1200</v>
-      </c>
-      <c r="Q11" s="65">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="67">
         <f>P11/Parâmetros!$B$1</f>
-        <v>5.4545454545454541</v>
-      </c>
-      <c r="R11" s="56">
+        <v>0</v>
+      </c>
+      <c r="R11" s="63">
         <f>Parâmetros!$B$2</f>
         <v>1.06</v>
       </c>
-      <c r="S11" s="56">
+      <c r="S11" s="63">
         <v>0.7</v>
       </c>
-      <c r="T11" s="56"/>
-      <c r="U11" s="65">
+      <c r="T11" s="63"/>
+      <c r="U11" s="67">
         <f>Q11/(R11*S11)</f>
-        <v>7.3511394266111241</v>
-      </c>
-      <c r="V11" s="56">
+        <v>0</v>
+      </c>
+      <c r="V11" s="63">
         <v>2.5</v>
       </c>
-      <c r="W11" s="56">
+      <c r="W11" s="63">
         <v>16</v>
       </c>
-      <c r="X11" s="56" t="s">
-        <v>53</v>
+      <c r="X11" s="63" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="28">
-        <f>Cômodos!B8</f>
-        <v>11.9</v>
-      </c>
-      <c r="E12" s="28">
-        <f>Cômodos!C8</f>
-        <v>15.2</v>
-      </c>
+      <c r="A12" s="66"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
-      <c r="J12" s="29">
-        <v>6</v>
-      </c>
-      <c r="K12" s="29">
-        <v>100</v>
-      </c>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
       <c r="L12" s="29">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M12" s="29"/>
       <c r="N12" s="29"/>
       <c r="O12" s="29"/>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="67"/>
-      <c r="R12" s="58"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="67"/>
-      <c r="V12" s="58"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="58"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="68"/>
+      <c r="R12" s="64"/>
+      <c r="S12" s="64"/>
+      <c r="T12" s="64"/>
+      <c r="U12" s="68"/>
+      <c r="V12" s="64"/>
+      <c r="W12" s="64"/>
+      <c r="X12" s="64"/>
     </row>
     <row r="13" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>7</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="19">
-        <f>Cômodos!B7</f>
-        <v>13.8</v>
-      </c>
-      <c r="E13" s="19">
-        <f>Cômodos!C7</f>
-        <v>15</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1">
-        <v>6</v>
-      </c>
-      <c r="K13" s="1">
-        <v>100</v>
-      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
       <c r="L13" s="1">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="14">
         <f>O13+L13</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="19">
         <f>P13/Parâmetros!$B$1</f>
-        <v>2.7272727272727271</v>
+        <v>0</v>
       </c>
       <c r="R13" s="1">
         <f>Parâmetros!$B$2</f>
@@ -1911,7 +1851,7 @@
       <c r="T13" s="1"/>
       <c r="U13" s="19">
         <f>Q13/(R13*S13)</f>
-        <v>3.675569713305562</v>
+        <v>0</v>
       </c>
       <c r="V13" s="1">
         <v>2.5</v>
@@ -1920,133 +1860,97 @@
         <v>16</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="68">
+      <c r="A14" s="76">
         <v>8</v>
       </c>
-      <c r="B14" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="37">
-        <f>Cômodos!B6</f>
-        <v>31.66</v>
-      </c>
-      <c r="E14" s="37">
-        <f>Cômodos!C6</f>
-        <v>30.32</v>
-      </c>
+      <c r="B14" s="69"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
       <c r="I14" s="36"/>
-      <c r="J14" s="36">
-        <v>11</v>
-      </c>
-      <c r="K14" s="36">
-        <v>100</v>
-      </c>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="36">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="M14" s="36"/>
       <c r="N14" s="36"/>
       <c r="O14" s="36"/>
-      <c r="P14" s="51">
+      <c r="P14" s="69">
         <f>L15+L14</f>
-        <v>1300</v>
-      </c>
-      <c r="Q14" s="70">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="71">
         <f>P14/Parâmetros!$B$1</f>
-        <v>5.9090909090909092</v>
-      </c>
-      <c r="R14" s="51">
+        <v>0</v>
+      </c>
+      <c r="R14" s="69">
         <f>Parâmetros!$B$2</f>
         <v>1.06</v>
       </c>
-      <c r="S14" s="51">
+      <c r="S14" s="69">
         <v>0.7</v>
       </c>
-      <c r="T14" s="51"/>
-      <c r="U14" s="70">
+      <c r="T14" s="69"/>
+      <c r="U14" s="71">
         <f t="shared" ref="U14" si="4">Q14/(R14*S14)</f>
-        <v>7.9637343788287183</v>
-      </c>
-      <c r="V14" s="51">
+        <v>0</v>
+      </c>
+      <c r="V14" s="69">
         <v>2.5</v>
       </c>
-      <c r="W14" s="51">
+      <c r="W14" s="69">
         <v>16</v>
       </c>
-      <c r="X14" s="51" t="s">
-        <v>52</v>
+      <c r="X14" s="69" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="69"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="37">
-        <f>Cômodos!B13</f>
-        <v>22.55</v>
-      </c>
-      <c r="E15" s="37">
-        <f>Cômodos!C13</f>
-        <v>24.7</v>
-      </c>
+      <c r="A15" s="77"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
       <c r="I15" s="36"/>
-      <c r="J15" s="36">
-        <v>2</v>
-      </c>
-      <c r="K15" s="36">
-        <v>100</v>
-      </c>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
       <c r="L15" s="36">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="M15" s="36"/>
       <c r="N15" s="36"/>
       <c r="O15" s="36"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="71"/>
-      <c r="R15" s="52"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="52"/>
-      <c r="U15" s="71"/>
-      <c r="V15" s="52"/>
-      <c r="W15" s="52"/>
-      <c r="X15" s="52"/>
+      <c r="P15" s="70"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="70"/>
+      <c r="S15" s="70"/>
+      <c r="T15" s="70"/>
+      <c r="U15" s="72"/>
+      <c r="V15" s="70"/>
+      <c r="W15" s="70"/>
+      <c r="X15" s="70"/>
     </row>
     <row r="16" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>9</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="19">
-        <f>Cômodos!B14</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="19">
-        <f>Cômodos!C14</f>
-        <v>0</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -2057,20 +1961,18 @@
       <c r="M16" s="1">
         <v>1</v>
       </c>
-      <c r="N16" s="1">
-        <v>8000</v>
-      </c>
+      <c r="N16" s="1"/>
       <c r="O16" s="1">
         <f>N16*M16</f>
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="P16" s="35">
         <f>O16+L16</f>
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="Q16" s="34">
         <f>P16/Parâmetros!B1</f>
-        <v>36.363636363636367</v>
+        <v>0</v>
       </c>
       <c r="R16" s="7">
         <f>Parâmetros!$B$2</f>
@@ -2082,7 +1984,7 @@
       <c r="T16" s="7"/>
       <c r="U16" s="34">
         <f>Q16/(R16*S16)</f>
-        <v>34.305317324185253</v>
+        <v>0</v>
       </c>
       <c r="V16" s="7">
         <v>10</v>
@@ -2091,40 +1993,26 @@
         <v>40</v>
       </c>
       <c r="X16" s="7" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="72">
+      <c r="A17" s="65">
         <v>10</v>
       </c>
-      <c r="B17" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="28">
-        <f>Cômodos!B13</f>
-        <v>22.55</v>
-      </c>
-      <c r="E17" s="28">
-        <f>Cômodos!C13</f>
-        <v>24.7</v>
-      </c>
-      <c r="F17" s="29">
-        <v>3</v>
-      </c>
-      <c r="G17" s="28">
-        <v>150</v>
-      </c>
+      <c r="B17" s="63"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="28"/>
       <c r="H17" s="29">
         <f>G17*F17</f>
-        <v>450</v>
-      </c>
-      <c r="I17" s="56">
+        <v>0</v>
+      </c>
+      <c r="I17" s="63">
         <f>SUM(H17:H23)</f>
-        <v>1230</v>
+        <v>0</v>
       </c>
       <c r="J17" s="29"/>
       <c r="K17" s="29"/>
@@ -2132,318 +2020,224 @@
       <c r="M17" s="29"/>
       <c r="N17" s="29"/>
       <c r="O17" s="29"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="65">
+      <c r="P17" s="63"/>
+      <c r="Q17" s="67">
         <f>I17/Parâmetros!$B$1</f>
-        <v>5.5909090909090908</v>
-      </c>
-      <c r="R17" s="56">
+        <v>0</v>
+      </c>
+      <c r="R17" s="63">
         <f>Parâmetros!$B$2</f>
         <v>1.06</v>
       </c>
-      <c r="S17" s="56">
+      <c r="S17" s="63">
         <v>0.7</v>
       </c>
-      <c r="T17" s="56"/>
-      <c r="U17" s="65">
+      <c r="T17" s="63"/>
+      <c r="U17" s="67">
         <f>Q17/(R17*S17)</f>
-        <v>7.534917912276403</v>
-      </c>
-      <c r="V17" s="56">
+        <v>0</v>
+      </c>
+      <c r="V17" s="63">
         <v>1.5</v>
       </c>
-      <c r="W17" s="56">
+      <c r="W17" s="63">
         <v>10</v>
       </c>
-      <c r="X17" s="56" t="s">
-        <v>51</v>
+      <c r="X17" s="63" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="73"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="28">
-        <f>Cômodos!B5</f>
-        <v>6</v>
-      </c>
-      <c r="E18" s="28">
-        <f>Cômodos!C5</f>
-        <v>10</v>
-      </c>
-      <c r="F18" s="29">
-        <v>1</v>
-      </c>
-      <c r="G18" s="28">
-        <f>Cômodos!D5</f>
-        <v>100</v>
-      </c>
+      <c r="A18" s="74"/>
+      <c r="B18" s="73"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="29">
         <f t="shared" ref="H18:H28" si="5">G18*F18</f>
-        <v>100</v>
-      </c>
-      <c r="I18" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="73"/>
       <c r="J18" s="29"/>
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
       <c r="N18" s="29"/>
       <c r="O18" s="29"/>
-      <c r="P18" s="57"/>
-      <c r="Q18" s="66"/>
-      <c r="R18" s="57"/>
-      <c r="S18" s="57"/>
-      <c r="T18" s="57"/>
-      <c r="U18" s="66"/>
-      <c r="V18" s="57"/>
-      <c r="W18" s="57"/>
-      <c r="X18" s="57"/>
+      <c r="P18" s="73"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="73"/>
+      <c r="S18" s="73"/>
+      <c r="T18" s="73"/>
+      <c r="U18" s="75"/>
+      <c r="V18" s="73"/>
+      <c r="W18" s="73"/>
+      <c r="X18" s="73"/>
     </row>
     <row r="19" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="28">
-        <f>Cômodos!B4</f>
-        <v>11.4</v>
-      </c>
-      <c r="E19" s="28">
-        <f>Cômodos!C4</f>
-        <v>13.7</v>
-      </c>
-      <c r="F19" s="29">
-        <v>1</v>
-      </c>
-      <c r="G19" s="28">
-        <f>Cômodos!D4</f>
-        <v>160</v>
-      </c>
+      <c r="A19" s="74"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="29">
         <f t="shared" si="5"/>
-        <v>160</v>
-      </c>
-      <c r="I19" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="73"/>
       <c r="J19" s="29"/>
       <c r="K19" s="29"/>
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
       <c r="N19" s="29"/>
       <c r="O19" s="29"/>
-      <c r="P19" s="57"/>
-      <c r="Q19" s="66"/>
-      <c r="R19" s="57"/>
-      <c r="S19" s="57"/>
-      <c r="T19" s="57"/>
-      <c r="U19" s="66"/>
-      <c r="V19" s="57"/>
-      <c r="W19" s="57"/>
-      <c r="X19" s="57"/>
+      <c r="P19" s="73"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="73"/>
+      <c r="S19" s="73"/>
+      <c r="T19" s="73"/>
+      <c r="U19" s="75"/>
+      <c r="V19" s="73"/>
+      <c r="W19" s="73"/>
+      <c r="X19" s="73"/>
     </row>
     <row r="20" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="28">
-        <f>Cômodos!B2</f>
-        <v>5.61</v>
-      </c>
-      <c r="E20" s="28">
-        <f>Cômodos!C2</f>
-        <v>9.91</v>
-      </c>
-      <c r="F20" s="29">
-        <v>1</v>
-      </c>
-      <c r="G20" s="28">
-        <f>Cômodos!D2</f>
-        <v>100</v>
-      </c>
+      <c r="A20" s="74"/>
+      <c r="B20" s="73"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="29">
         <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="I20" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="73"/>
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
       <c r="L20" s="29"/>
       <c r="M20" s="29"/>
       <c r="N20" s="29"/>
       <c r="O20" s="29"/>
-      <c r="P20" s="57"/>
-      <c r="Q20" s="66"/>
-      <c r="R20" s="57"/>
-      <c r="S20" s="57"/>
-      <c r="T20" s="57"/>
-      <c r="U20" s="66"/>
-      <c r="V20" s="57"/>
-      <c r="W20" s="57"/>
-      <c r="X20" s="57"/>
+      <c r="P20" s="73"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="73"/>
+      <c r="S20" s="73"/>
+      <c r="T20" s="73"/>
+      <c r="U20" s="75"/>
+      <c r="V20" s="73"/>
+      <c r="W20" s="73"/>
+      <c r="X20" s="73"/>
     </row>
     <row r="21" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="73"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="28">
-        <f>Cômodos!B3</f>
-        <v>5.36</v>
-      </c>
-      <c r="E21" s="28">
-        <f>Cômodos!C3</f>
-        <v>9.76</v>
-      </c>
-      <c r="F21" s="29">
-        <v>1</v>
-      </c>
-      <c r="G21" s="28">
-        <f>Cômodos!D3</f>
-        <v>100</v>
-      </c>
+      <c r="A21" s="74"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="29">
         <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="I21" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="73"/>
       <c r="J21" s="29"/>
       <c r="K21" s="29"/>
       <c r="L21" s="29"/>
       <c r="M21" s="29"/>
       <c r="N21" s="29"/>
       <c r="O21" s="29"/>
-      <c r="P21" s="57"/>
-      <c r="Q21" s="66"/>
-      <c r="R21" s="57"/>
-      <c r="S21" s="57"/>
-      <c r="T21" s="57"/>
-      <c r="U21" s="66"/>
-      <c r="V21" s="57"/>
-      <c r="W21" s="57"/>
-      <c r="X21" s="57"/>
+      <c r="P21" s="73"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="73"/>
+      <c r="S21" s="73"/>
+      <c r="T21" s="73"/>
+      <c r="U21" s="75"/>
+      <c r="V21" s="73"/>
+      <c r="W21" s="73"/>
+      <c r="X21" s="73"/>
     </row>
     <row r="22" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="28">
-        <f>Cômodos!B9</f>
-        <v>17</v>
-      </c>
-      <c r="E22" s="28">
-        <f>Cômodos!C9</f>
-        <v>16.899999999999999</v>
-      </c>
-      <c r="F22" s="29">
-        <v>1</v>
-      </c>
-      <c r="G22" s="28">
-        <f>Cômodos!D9</f>
-        <v>220</v>
-      </c>
+      <c r="A22" s="74"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="29">
         <f t="shared" si="5"/>
-        <v>220</v>
-      </c>
-      <c r="I22" s="57"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="73"/>
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
       <c r="L22" s="29"/>
       <c r="M22" s="29"/>
       <c r="N22" s="29"/>
       <c r="O22" s="29"/>
-      <c r="P22" s="57"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="57"/>
-      <c r="S22" s="57"/>
-      <c r="T22" s="57"/>
-      <c r="U22" s="66"/>
-      <c r="V22" s="57"/>
-      <c r="W22" s="57"/>
-      <c r="X22" s="57"/>
+      <c r="P22" s="73"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="73"/>
+      <c r="S22" s="73"/>
+      <c r="T22" s="73"/>
+      <c r="U22" s="75"/>
+      <c r="V22" s="73"/>
+      <c r="W22" s="73"/>
+      <c r="X22" s="73"/>
     </row>
     <row r="23" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="74"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="28">
-        <f>Cômodos!B12</f>
-        <v>6.42</v>
-      </c>
-      <c r="E23" s="28">
-        <f>Cômodos!C12</f>
-        <v>12.2</v>
-      </c>
-      <c r="F23" s="29">
-        <v>1</v>
-      </c>
-      <c r="G23" s="28">
-        <f>Cômodos!D12</f>
-        <v>100</v>
-      </c>
+      <c r="A23" s="66"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="29">
         <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-      <c r="I23" s="58"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="64"/>
       <c r="J23" s="29"/>
       <c r="K23" s="29"/>
       <c r="L23" s="29"/>
       <c r="M23" s="29"/>
       <c r="N23" s="29"/>
       <c r="O23" s="29"/>
-      <c r="P23" s="58"/>
-      <c r="Q23" s="67"/>
-      <c r="R23" s="58"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="58"/>
-      <c r="U23" s="67"/>
-      <c r="V23" s="58"/>
-      <c r="W23" s="58"/>
-      <c r="X23" s="58"/>
+      <c r="P23" s="64"/>
+      <c r="Q23" s="68"/>
+      <c r="R23" s="64"/>
+      <c r="S23" s="64"/>
+      <c r="T23" s="64"/>
+      <c r="U23" s="68"/>
+      <c r="V23" s="64"/>
+      <c r="W23" s="64"/>
+      <c r="X23" s="64"/>
     </row>
     <row r="24" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="62">
+      <c r="A24" s="56">
         <v>11</v>
       </c>
-      <c r="B24" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="1" t="str">
-        <f>Cômodos!A10</f>
-        <v>Circulação</v>
-      </c>
-      <c r="D24" s="1">
-        <f>Cômodos!B10</f>
-        <v>8.5</v>
-      </c>
-      <c r="E24" s="1">
-        <f>Cômodos!C10</f>
-        <v>13.25</v>
-      </c>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1">
-        <f>Cômodos!D10</f>
-        <v>100</v>
-      </c>
+      <c r="B24" s="53"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
       <c r="H24" s="1">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I24" s="53">
         <f>SUM(H24:H28)</f>
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -2454,7 +2248,7 @@
       <c r="P24" s="53"/>
       <c r="Q24" s="59">
         <f>I24/Parâmetros!$B$1</f>
-        <v>4.6363636363636367</v>
+        <v>0</v>
       </c>
       <c r="R24" s="53">
         <f>Parâmetros!$B$2</f>
@@ -2466,7 +2260,7 @@
       <c r="T24" s="53"/>
       <c r="U24" s="59">
         <f>Q24/(R24*S24)</f>
-        <v>6.2484685126194561</v>
+        <v>0</v>
       </c>
       <c r="V24" s="53">
         <v>1.5</v>
@@ -2475,34 +2269,20 @@
         <v>10</v>
       </c>
       <c r="X24" s="53" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="63"/>
+      <c r="A25" s="57"/>
       <c r="B25" s="54"/>
-      <c r="C25" s="19" t="str">
-        <f>Cômodos!A8</f>
-        <v>Quarto 2</v>
-      </c>
-      <c r="D25" s="19">
-        <f>Cômodos!B8</f>
-        <v>11.9</v>
-      </c>
-      <c r="E25" s="19">
-        <f>Cômodos!C8</f>
-        <v>15.2</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="19">
-        <f>Cômodos!D8</f>
-        <v>160</v>
-      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="19"/>
       <c r="H25" s="1">
         <f t="shared" si="5"/>
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="I25" s="54"/>
       <c r="J25" s="1"/>
@@ -2522,30 +2302,16 @@
       <c r="X25" s="54"/>
     </row>
     <row r="26" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="63"/>
+      <c r="A26" s="57"/>
       <c r="B26" s="54"/>
-      <c r="C26" s="1" t="str">
-        <f>Cômodos!A7</f>
-        <v>Quarto 1</v>
-      </c>
-      <c r="D26" s="1">
-        <f>Cômodos!B7</f>
-        <v>13.8</v>
-      </c>
-      <c r="E26" s="1">
-        <f>Cômodos!C7</f>
-        <v>15</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1">
-        <f>Cômodos!D7</f>
-        <v>160</v>
-      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
       <c r="H26" s="1">
         <f t="shared" si="5"/>
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="I26" s="54"/>
       <c r="J26" s="1"/>
@@ -2565,30 +2331,16 @@
       <c r="X26" s="54"/>
     </row>
     <row r="27" spans="1:24" s="30" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="63"/>
+      <c r="A27" s="57"/>
       <c r="B27" s="54"/>
-      <c r="C27" s="1" t="str">
-        <f>Cômodos!A11</f>
-        <v>Varanda Q1</v>
-      </c>
-      <c r="D27" s="1">
-        <f>Cômodos!B11</f>
-        <v>6.73</v>
-      </c>
-      <c r="E27" s="1">
-        <f>Cômodos!C11</f>
-        <v>13.09</v>
-      </c>
-      <c r="F27" s="1">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1">
-        <f>Cômodos!D11</f>
-        <v>100</v>
-      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
       <c r="H27" s="1">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I27" s="54"/>
       <c r="J27" s="1"/>
@@ -2608,29 +2360,16 @@
       <c r="X27" s="54"/>
     </row>
     <row r="28" spans="1:24" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="64"/>
+      <c r="A28" s="58"/>
       <c r="B28" s="55"/>
-      <c r="C28" s="1" t="str">
-        <f>Cômodos!A6</f>
-        <v>Sala</v>
-      </c>
-      <c r="D28" s="1">
-        <f>Cômodos!B6</f>
-        <v>31.66</v>
-      </c>
-      <c r="E28" s="1">
-        <f>Cômodos!C6</f>
-        <v>30.32</v>
-      </c>
-      <c r="F28" s="1">
-        <v>2</v>
-      </c>
-      <c r="G28" s="1">
-        <v>250</v>
-      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
       <c r="H28" s="1">
         <f t="shared" si="5"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="I28" s="55"/>
       <c r="J28" s="1"/>
@@ -2653,27 +2392,19 @@
       <c r="A29" s="39">
         <v>12</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1">
-        <v>6</v>
-      </c>
-      <c r="G29" s="1">
-        <v>150</v>
-      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
       <c r="H29" s="1">
         <f t="shared" ref="H29" si="6">G29*F29</f>
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="I29" s="7">
         <f>SUM(H29:H29)</f>
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2684,7 +2415,7 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="34">
         <f>I29/Parâmetros!$B$1</f>
-        <v>4.0909090909090908</v>
+        <v>0</v>
       </c>
       <c r="R29" s="7">
         <f>Parâmetros!$B$2</f>
@@ -2696,7 +2427,7 @@
       <c r="T29" s="7"/>
       <c r="U29" s="34">
         <f>Q29/(R29*S29)</f>
-        <v>3.85934819897084</v>
+        <v>0</v>
       </c>
       <c r="V29" s="7">
         <v>1.5</v>
@@ -2705,7 +2436,7 @@
         <v>10</v>
       </c>
       <c r="X29" s="7" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
@@ -2753,18 +2484,18 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1">
         <f t="shared" ref="P31" si="7">SUM(P4:P28)</f>
-        <v>36800</v>
+        <v>7900</v>
       </c>
       <c r="Q31" s="19">
         <f>SUM(Q4:Q29)</f>
-        <v>181.59090909090909</v>
+        <v>35.909090909090914</v>
       </c>
       <c r="R31" s="19"/>
       <c r="S31" s="40"/>
       <c r="T31" s="19"/>
       <c r="U31" s="19">
         <f>SUM(U4:U29)</f>
-        <v>188.67924528301887</v>
+        <v>41.043861798578781</v>
       </c>
       <c r="V31" s="41"/>
       <c r="W31" s="1"/>
@@ -2790,11 +2521,11 @@
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
       <c r="T32" s="32" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="U32" s="1">
         <f>U31*Parâmetros!B1</f>
-        <v>41509.433962264149</v>
+        <v>9029.6495956873314</v>
       </c>
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
@@ -2952,6 +2683,60 @@
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="W14:W15"/>
+    <mergeCell ref="U17:U23"/>
+    <mergeCell ref="X14:X15"/>
+    <mergeCell ref="W24:W28"/>
+    <mergeCell ref="X24:X28"/>
+    <mergeCell ref="V17:V23"/>
+    <mergeCell ref="W17:W23"/>
+    <mergeCell ref="X17:X23"/>
+    <mergeCell ref="R24:R28"/>
+    <mergeCell ref="S24:S28"/>
+    <mergeCell ref="T24:T28"/>
+    <mergeCell ref="U24:U28"/>
+    <mergeCell ref="V24:V28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="I24:I28"/>
+    <mergeCell ref="P24:P28"/>
+    <mergeCell ref="Q24:Q28"/>
+    <mergeCell ref="S14:S15"/>
+    <mergeCell ref="T14:T15"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="T17:T23"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="I17:I23"/>
+    <mergeCell ref="B17:B23"/>
+    <mergeCell ref="Q17:Q23"/>
+    <mergeCell ref="P17:P23"/>
+    <mergeCell ref="R17:R23"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="S17:S23"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="W11:W12"/>
+    <mergeCell ref="X11:X12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="S11:S12"/>
+    <mergeCell ref="T11:T12"/>
+    <mergeCell ref="W8:W10"/>
+    <mergeCell ref="X8:X10"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="V2:V3"/>
     <mergeCell ref="S8:S10"/>
@@ -2968,60 +2753,6 @@
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="P2:P3"/>
-    <mergeCell ref="W8:W10"/>
-    <mergeCell ref="X8:X10"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="V11:V12"/>
-    <mergeCell ref="W11:W12"/>
-    <mergeCell ref="X11:X12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="T11:T12"/>
-    <mergeCell ref="S14:S15"/>
-    <mergeCell ref="T14:T15"/>
-    <mergeCell ref="U14:U15"/>
-    <mergeCell ref="T17:T23"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="I17:I23"/>
-    <mergeCell ref="B17:B23"/>
-    <mergeCell ref="Q17:Q23"/>
-    <mergeCell ref="P17:P23"/>
-    <mergeCell ref="R17:R23"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="Q14:Q15"/>
-    <mergeCell ref="R14:R15"/>
-    <mergeCell ref="S17:S23"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="I24:I28"/>
-    <mergeCell ref="P24:P28"/>
-    <mergeCell ref="Q24:Q28"/>
-    <mergeCell ref="R24:R28"/>
-    <mergeCell ref="S24:S28"/>
-    <mergeCell ref="T24:T28"/>
-    <mergeCell ref="U24:U28"/>
-    <mergeCell ref="V24:V28"/>
-    <mergeCell ref="V14:V15"/>
-    <mergeCell ref="W14:W15"/>
-    <mergeCell ref="U17:U23"/>
-    <mergeCell ref="X14:X15"/>
-    <mergeCell ref="W24:W28"/>
-    <mergeCell ref="X24:X28"/>
-    <mergeCell ref="V17:V23"/>
-    <mergeCell ref="W17:W23"/>
-    <mergeCell ref="X17:X23"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.563194444444444" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="8" scale="74" fitToWidth="0" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3033,11 +2764,236 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310492F5-C5D9-4BB0-96E1-BE93A7943BC8}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="A1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.21875" customWidth="1"/>
+    <col min="6" max="7" width="21.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="81" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+    </row>
+    <row r="2" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+    </row>
+    <row r="3" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="80" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+    </row>
+    <row r="4" spans="1:5" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+    </row>
+    <row r="5" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+    </row>
+    <row r="6" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+    </row>
+    <row r="7" spans="1:5" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="79" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="79" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="80"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+    </row>
+    <row r="9" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="79"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+    </row>
+    <row r="10" spans="1:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="78"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="78"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="78"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="78"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="81" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="80">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="80">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="80">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="80">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="79" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="80">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="79" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="80">
+        <f>SUM(B15:B19)</f>
+        <v>1980</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{F46712CA-43A2-46FD-A796-763BEF2C7A93}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{6C62D24E-D37B-4A7E-BE62-AC15AF946261}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{F4988C85-937B-4CE5-8C95-53BA00A5E86A}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{790F3034-2945-4553-ACD2-8CB7BB3BA80E}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F1FE56B-3B6F-42C2-8CC7-CC59AB53DE6D}">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3050,77 +3006,77 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="45" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B2" s="46">
         <f>SUM('Quadro de cargas'!U17:U29)*Parâmetros!B1</f>
-        <v>3881.4016172506736</v>
+        <v>0</v>
       </c>
       <c r="C2" s="47">
         <v>0.59</v>
       </c>
       <c r="D2" s="46">
         <f>C2*B2</f>
-        <v>2290.0269541778971</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="45" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B3" s="46">
         <f>(SUM('Quadro de cargas'!U6:U16)-'Quadro de cargas'!U16)*Parâmetros!B1</f>
-        <v>16118.598382749326</v>
+        <v>9029.6495956873314</v>
       </c>
       <c r="C3" s="47">
         <v>0.24</v>
       </c>
       <c r="D3" s="46">
         <f t="shared" ref="D3" si="0">C3*B3</f>
-        <v>3868.4636118598378</v>
+        <v>2167.1159029649593</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B4" s="46">
         <f>SUM('Quadro de cargas'!U4:U5)*Parâmetros!B1</f>
-        <v>13962.264150943394</v>
+        <v>0</v>
       </c>
       <c r="C4" s="47">
         <v>1</v>
       </c>
       <c r="D4" s="46">
         <f>C4*B4</f>
-        <v>13962.264150943394</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B5" s="46">
         <f>'Quadro de cargas'!U16*Parâmetros!B1</f>
-        <v>7547.1698113207558</v>
+        <v>0</v>
       </c>
       <c r="C5" s="47">
         <v>1</v>
       </c>
       <c r="D5" s="46">
         <f>C5*B5</f>
-        <v>7547.1698113207558</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3136,33 +3092,33 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="43"/>
       <c r="C8" s="48" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D8" s="46">
         <f>SUM(D2:D6)</f>
-        <v>27667.924528301886</v>
+        <v>2167.1159029649593</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="45" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="D9" s="49">
         <f>D8/(Parâmetros!B3*SQRT(3))</f>
-        <v>42.037062300877224</v>
+        <v>3.2925919735314166</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="45" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="45" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D12" s="49">
         <v>5.0999999999999996</v>
@@ -3170,7 +3126,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="45" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D13" s="49">
         <v>4</v>
@@ -3178,7 +3134,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="45" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D14" s="49">
         <f>3.1415*(D12/2)^2*D13</f>
@@ -3187,7 +3143,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="45" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D16" s="49">
         <v>1</v>
@@ -3195,7 +3151,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" s="45" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D17" s="49">
         <f>3.1415*((D16*25.4)/2)^2</f>
@@ -3204,7 +3160,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" s="45" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D18" s="50">
         <f>D14/D17</f>
@@ -3219,12 +3175,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80942C2F-3B43-4C64-AE6D-0AB05219C999}">
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3237,255 +3193,128 @@
   <sheetData>
     <row r="1" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>43</v>
-      </c>
       <c r="E1" s="17" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="19">
-        <v>5.61</v>
-      </c>
-      <c r="C2" s="19">
-        <v>9.91</v>
-      </c>
-      <c r="D2" s="19">
-        <v>100</v>
-      </c>
-      <c r="E2" s="19">
-        <v>3</v>
-      </c>
+      <c r="A2" s="14"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="20"/>
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="19">
-        <v>5.36</v>
-      </c>
-      <c r="C3" s="19">
-        <v>9.76</v>
-      </c>
-      <c r="D3" s="19">
-        <v>100</v>
-      </c>
-      <c r="E3" s="19">
-        <v>3</v>
-      </c>
+      <c r="A3" s="14"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="20"/>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="19">
-        <v>11.4</v>
-      </c>
-      <c r="C4" s="19">
-        <v>13.7</v>
-      </c>
-      <c r="D4" s="19">
-        <v>160</v>
-      </c>
-      <c r="E4" s="19">
-        <f>ROUND(C4/3.5,0)*1</f>
-        <v>4</v>
-      </c>
+      <c r="A4" s="14"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="19">
-        <v>6</v>
-      </c>
-      <c r="C5" s="19">
-        <v>10</v>
-      </c>
-      <c r="D5" s="19">
-        <v>100</v>
-      </c>
-      <c r="E5" s="19">
-        <f>ROUND(C5/3.5,0)*1</f>
-        <v>3</v>
-      </c>
+      <c r="A5" s="14"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="19">
-        <v>31.66</v>
-      </c>
-      <c r="C6" s="19">
-        <v>30.32</v>
-      </c>
-      <c r="D6" s="19">
-        <f>ROUNDDOWN((31.66-6)/4,0)*60+100</f>
-        <v>460</v>
-      </c>
-      <c r="E6" s="19">
-        <f>ROUND(C6/5,0)*1</f>
-        <v>6</v>
-      </c>
+      <c r="A6" s="14"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="19">
-        <v>13.8</v>
-      </c>
-      <c r="C7" s="19">
-        <v>15</v>
-      </c>
-      <c r="D7" s="19">
-        <v>160</v>
-      </c>
-      <c r="E7" s="19">
-        <f t="shared" ref="E7:E9" si="0">ROUND(C7/5,0)*1</f>
-        <v>3</v>
-      </c>
+      <c r="A7" s="14"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="21">
-        <v>11.9</v>
-      </c>
-      <c r="C8" s="19">
-        <v>15.2</v>
-      </c>
-      <c r="D8" s="19">
-        <v>160</v>
-      </c>
-      <c r="E8" s="19">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="A8" s="14"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="20"/>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="21">
-        <v>17</v>
-      </c>
-      <c r="C9" s="21">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="D9" s="21">
-        <v>220</v>
-      </c>
-      <c r="E9" s="19">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="A9" s="22"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="19"/>
       <c r="F9" s="21"/>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="21">
-        <v>8.5</v>
-      </c>
-      <c r="C10" s="21">
-        <v>13.25</v>
-      </c>
-      <c r="D10" s="21">
-        <v>100</v>
-      </c>
-      <c r="E10" s="19">
-        <v>1</v>
-      </c>
+      <c r="A10" s="22"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="21"/>
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="21">
-        <v>6.73</v>
-      </c>
-      <c r="C11" s="21">
-        <v>13.09</v>
-      </c>
-      <c r="D11" s="21">
-        <v>100</v>
-      </c>
-      <c r="E11" s="21">
-        <v>1</v>
-      </c>
+      <c r="A11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="21">
-        <v>6.42</v>
-      </c>
-      <c r="C12" s="21">
-        <v>12.2</v>
-      </c>
-      <c r="D12" s="21">
-        <v>100</v>
-      </c>
-      <c r="E12" s="21">
-        <v>1</v>
-      </c>
+      <c r="A12" s="22"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="21"/>
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="21">
-        <v>22.55</v>
-      </c>
-      <c r="C13" s="21">
-        <v>24.7</v>
-      </c>
-      <c r="D13" s="21">
-        <v>340</v>
-      </c>
-      <c r="E13" s="21">
-        <v>1</v>
-      </c>
+      <c r="A13" s="22"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="21"/>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
@@ -3604,7 +3433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E87ADD-43D1-45EA-813E-8C2EE7F75743}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3616,7 +3445,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B1">
         <v>220</v>
@@ -3632,7 +3461,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>380</v>
@@ -3643,7 +3472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B241DD-D43C-40E0-9FBA-E2F87E7EF9B7}">
   <dimension ref="G25"/>
   <sheetViews>
@@ -3655,7 +3484,7 @@
   <sheetData>
     <row r="25" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Condutores desenhados, com apenas uma linha de montagem
</commit_message>
<xml_diff>
--- a/Quadro de cargas - Maquinas.xlsx
+++ b/Quadro de cargas - Maquinas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\Documents\Giovani\UCS\Instalações Elétricas (2)\UCS_Projeto_Instala-es_Industriais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9B7493-EC11-4755-9EB7-71331DC616E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA57FD6-F538-443F-A73E-754EABB66814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2475" windowWidth="20640" windowHeight="11760" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="120">
   <si>
     <t>Cargas de Iluminação</t>
   </si>
@@ -317,9 +317,6 @@
     <t>Forno refusão 1</t>
   </si>
   <si>
-    <t>Forno refusão 2</t>
-  </si>
-  <si>
     <t>Ohms/m</t>
   </si>
   <si>
@@ -332,9 +329,6 @@
     <t>Printer 1</t>
   </si>
   <si>
-    <t>Printer 2</t>
-  </si>
-  <si>
     <t>Conveyor 1</t>
   </si>
   <si>
@@ -344,25 +338,10 @@
     <t>Pick and place 2</t>
   </si>
   <si>
-    <t>Pick and place 3</t>
-  </si>
-  <si>
     <t>Conveyor 2</t>
   </si>
   <si>
-    <t>Pick and place 4</t>
-  </si>
-  <si>
-    <t>Conveyor 3</t>
-  </si>
-  <si>
-    <t>Conveyor 4</t>
-  </si>
-  <si>
     <t>AOI 1</t>
-  </si>
-  <si>
-    <t>AOI 2</t>
   </si>
   <si>
     <t>Wave solder</t>
@@ -1297,11 +1276,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1311,17 +1290,8 @@
     <col min="3" max="3" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16" width="8.21875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.88671875" style="1" customWidth="1"/>
     <col min="18" max="18" width="6.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
@@ -1399,7 +1369,7 @@
         <v>18</v>
       </c>
       <c r="U2" s="50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V2" s="50" t="s">
         <v>5</v>
@@ -1479,7 +1449,7 @@
         <v>82</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D4" s="16">
         <f>11.3*22.8</f>
@@ -1538,7 +1508,7 @@
         <v>100</v>
       </c>
       <c r="Y4" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1546,17 +1516,17 @@
         <v>2</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D5" s="16">
-        <f>11.3*22.8</f>
+        <f t="shared" ref="D5:D12" si="0">11.3*22.8</f>
         <v>257.64000000000004</v>
       </c>
       <c r="E5" s="16">
-        <f>11.3*2+22.8*2</f>
+        <f t="shared" ref="E5:E12" si="1">11.3*2+22.8*2</f>
         <v>68.2</v>
       </c>
       <c r="F5" s="41"/>
@@ -1570,18 +1540,19 @@
         <v>1</v>
       </c>
       <c r="N5" s="41">
-        <v>68000</v>
+        <v>2000</v>
       </c>
       <c r="O5" s="41">
         <f>N5*M5</f>
-        <v>68000</v>
+        <v>2000</v>
       </c>
       <c r="P5" s="12">
-        <v>60000</v>
+        <f>O5+L5</f>
+        <v>2000</v>
       </c>
       <c r="Q5" s="16">
-        <f>P5/(SQRT(3)*380)</f>
-        <v>91.160568819414607</v>
+        <f>P5/220</f>
+        <v>9.0909090909090917</v>
       </c>
       <c r="R5" s="41">
         <f>Parâmetros!$B$2</f>
@@ -1594,21 +1565,21 @@
         <v>30</v>
       </c>
       <c r="U5" s="16">
-        <f>(T5*Maquinas!$D$5)*'Quadro de cargas'!V5</f>
-        <v>1.4293289186591231</v>
+        <f>(T5*Maquinas!$H$12)*'Quadro de cargas'!V5</f>
+        <v>2.1123499142367073</v>
       </c>
       <c r="V5" s="16">
-        <f>Q5/(R5*S5)</f>
-        <v>86.000536622089243</v>
+        <f t="shared" ref="V5:V24" si="2">Q5/(R5*S5)</f>
+        <v>8.5763293310463133</v>
       </c>
       <c r="W5" s="41">
-        <v>35</v>
+        <v>2.5</v>
       </c>
       <c r="X5" s="41">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="Y5" s="41" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1619,40 +1590,43 @@
         <v>87</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D6" s="16">
-        <f t="shared" ref="D6:D19" si="0">11.3*22.8</f>
+        <f t="shared" si="0"/>
         <v>257.64000000000004</v>
       </c>
       <c r="E6" s="16">
-        <f t="shared" ref="E6:E19" si="1">11.3*2+22.8*2</f>
+        <f t="shared" si="1"/>
         <v>68.2</v>
       </c>
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
       <c r="I6" s="12"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41">
+      <c r="J6" s="41">
         <v>1</v>
       </c>
-      <c r="N6" s="41">
-        <v>2000</v>
-      </c>
+      <c r="K6" s="41">
+        <v>150</v>
+      </c>
+      <c r="L6" s="41">
+        <f>K6*J6</f>
+        <v>150</v>
+      </c>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
       <c r="O6" s="41">
-        <f>N6*M6</f>
-        <v>2000</v>
+        <f t="shared" ref="O6:O8" si="3">N6*M6</f>
+        <v>0</v>
       </c>
       <c r="P6" s="12">
-        <f>O6+L6</f>
-        <v>2000</v>
+        <f t="shared" ref="P6:P8" si="4">O6+L6</f>
+        <v>150</v>
       </c>
       <c r="Q6" s="16">
         <f>P6/220</f>
-        <v>9.0909090909090917</v>
+        <v>0.68181818181818177</v>
       </c>
       <c r="R6" s="41">
         <f>Parâmetros!$B$2</f>
@@ -1662,15 +1636,15 @@
         <v>1</v>
       </c>
       <c r="T6" s="41">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="U6" s="16">
         <f>(T6*Maquinas!$H$12)*'Quadro de cargas'!V6</f>
-        <v>2.1123499142367073</v>
+        <v>7.9213121783876489E-2</v>
       </c>
       <c r="V6" s="16">
-        <f t="shared" ref="V6:V31" si="2">Q6/(R6*S6)</f>
-        <v>8.5763293310463133</v>
+        <f t="shared" si="2"/>
+        <v>0.6432246998284733</v>
       </c>
       <c r="W6" s="41">
         <v>2.5</v>
@@ -1679,7 +1653,7 @@
         <v>16</v>
       </c>
       <c r="Y6" s="41" t="s">
-        <v>114</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1687,10 +1661,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
@@ -1704,26 +1678,29 @@
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
       <c r="I7" s="12"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41">
+      <c r="J7" s="41">
         <v>1</v>
       </c>
-      <c r="N7" s="41">
-        <v>2000</v>
-      </c>
+      <c r="K7" s="41">
+        <v>150</v>
+      </c>
+      <c r="L7" s="41">
+        <f t="shared" ref="L7:L10" si="5">K7*J7</f>
+        <v>150</v>
+      </c>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
       <c r="O7" s="41">
-        <f t="shared" ref="O7:O12" si="3">N7*M7</f>
-        <v>2000</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="P7" s="12">
-        <f t="shared" ref="P7:P12" si="4">O7+L7</f>
-        <v>2000</v>
+        <f t="shared" si="4"/>
+        <v>150</v>
       </c>
       <c r="Q7" s="16">
-        <f>P7/220</f>
-        <v>9.0909090909090917</v>
+        <f t="shared" ref="Q7" si="6">P7/220</f>
+        <v>0.68181818181818177</v>
       </c>
       <c r="R7" s="41">
         <f>Parâmetros!$B$2</f>
@@ -1737,11 +1714,11 @@
       </c>
       <c r="U7" s="16">
         <f>(T7*Maquinas!$H$12)*'Quadro de cargas'!V7</f>
-        <v>2.1123499142367073</v>
+        <v>0.15842624356775298</v>
       </c>
       <c r="V7" s="16">
         <f t="shared" si="2"/>
-        <v>8.5763293310463133</v>
+        <v>0.6432246998284733</v>
       </c>
       <c r="W7" s="41">
         <v>2.5</v>
@@ -1750,7 +1727,7 @@
         <v>16</v>
       </c>
       <c r="Y7" s="41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1758,10 +1735,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D8" s="16">
         <f t="shared" si="0"/>
@@ -1775,29 +1752,29 @@
       <c r="G8" s="41"/>
       <c r="H8" s="41"/>
       <c r="I8" s="12"/>
-      <c r="J8" s="41">
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="41">
         <v>1</v>
       </c>
-      <c r="K8" s="41">
-        <v>150</v>
-      </c>
-      <c r="L8" s="41">
-        <f>K8*J8</f>
-        <v>150</v>
-      </c>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
+      <c r="N8" s="41">
+        <v>2500</v>
+      </c>
       <c r="O8" s="41">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="P8" s="12">
         <f t="shared" si="4"/>
-        <v>150</v>
+        <v>2500</v>
       </c>
       <c r="Q8" s="16">
-        <f>P8/220</f>
-        <v>0.68181818181818177</v>
+        <f>P8/(SQRT(3)*380)</f>
+        <v>3.798357034142275</v>
       </c>
       <c r="R8" s="41">
         <f>Parâmetros!$B$2</f>
@@ -1807,15 +1784,15 @@
         <v>1</v>
       </c>
       <c r="T8" s="41">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="U8" s="16">
         <f>(T8*Maquinas!$H$12)*'Quadro de cargas'!V8</f>
-        <v>7.9213121783876489E-2</v>
+        <v>0.58838700472279393</v>
       </c>
       <c r="V8" s="16">
         <f t="shared" si="2"/>
-        <v>0.6432246998284733</v>
+        <v>3.5833556925870518</v>
       </c>
       <c r="W8" s="41">
         <v>2.5</v>
@@ -1824,7 +1801,7 @@
         <v>16</v>
       </c>
       <c r="Y8" s="41" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1832,10 +1809,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="0"/>
@@ -1849,29 +1826,29 @@
       <c r="G9" s="41"/>
       <c r="H9" s="41"/>
       <c r="I9" s="12"/>
-      <c r="J9" s="41">
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="41">
         <v>1</v>
       </c>
-      <c r="K9" s="41">
-        <v>150</v>
-      </c>
-      <c r="L9" s="41">
-        <f t="shared" ref="L9:L16" si="5">K9*J9</f>
-        <v>150</v>
-      </c>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
+      <c r="N9" s="41">
+        <v>2500</v>
+      </c>
       <c r="O9" s="41">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="O9" si="7">N9*M9</f>
+        <v>2500</v>
       </c>
       <c r="P9" s="12">
-        <f t="shared" si="4"/>
-        <v>150</v>
+        <f t="shared" ref="P9:P10" si="8">O9+L9</f>
+        <v>2500</v>
       </c>
       <c r="Q9" s="16">
-        <f t="shared" ref="Q9:Q11" si="6">P9/220</f>
-        <v>0.68181818181818177</v>
+        <f t="shared" ref="Q9" si="9">P9/(SQRT(3)*380)</f>
+        <v>3.798357034142275</v>
       </c>
       <c r="R9" s="41">
         <f>Parâmetros!$B$2</f>
@@ -1881,15 +1858,15 @@
         <v>1</v>
       </c>
       <c r="T9" s="41">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="U9" s="16">
         <f>(T9*Maquinas!$H$12)*'Quadro de cargas'!V9</f>
-        <v>0.15842624356775298</v>
+        <v>0.58838700472279393</v>
       </c>
       <c r="V9" s="16">
         <f t="shared" si="2"/>
-        <v>0.6432246998284733</v>
+        <v>3.5833556925870518</v>
       </c>
       <c r="W9" s="41">
         <v>2.5</v>
@@ -1898,7 +1875,7 @@
         <v>16</v>
       </c>
       <c r="Y9" s="41" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1906,10 +1883,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" si="0"/>
@@ -1923,29 +1900,30 @@
       <c r="G10" s="41"/>
       <c r="H10" s="41"/>
       <c r="I10" s="12"/>
-      <c r="J10" s="41">
-        <v>1</v>
-      </c>
-      <c r="K10" s="41">
-        <v>150</v>
-      </c>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
       <c r="L10" s="41">
         <f t="shared" si="5"/>
-        <v>150</v>
-      </c>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="41">
+        <v>1</v>
+      </c>
+      <c r="N10" s="41">
+        <f>220*8</f>
+        <v>1760</v>
+      </c>
       <c r="O10" s="41">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>N10*M10</f>
+        <v>1760</v>
       </c>
       <c r="P10" s="12">
-        <f t="shared" si="4"/>
-        <v>150</v>
+        <f t="shared" si="8"/>
+        <v>1760</v>
       </c>
       <c r="Q10" s="16">
-        <f t="shared" si="6"/>
-        <v>0.68181818181818177</v>
+        <f>P10/220</f>
+        <v>8</v>
       </c>
       <c r="R10" s="41">
         <f>Parâmetros!$B$2</f>
@@ -1955,15 +1933,15 @@
         <v>1</v>
       </c>
       <c r="T10" s="41">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="U10" s="16">
         <f>(T10*Maquinas!$H$12)*'Quadro de cargas'!V10</f>
-        <v>0.10561749571183532</v>
+        <v>1.5490566037735849</v>
       </c>
       <c r="V10" s="16">
-        <f t="shared" si="2"/>
-        <v>0.6432246998284733</v>
+        <f>Q10/(R10*S10)</f>
+        <v>7.5471698113207539</v>
       </c>
       <c r="W10" s="41">
         <v>2.5</v>
@@ -1972,7 +1950,7 @@
         <v>16</v>
       </c>
       <c r="Y10" s="41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1980,10 +1958,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="0"/>
@@ -1997,29 +1975,26 @@
       <c r="G11" s="41"/>
       <c r="H11" s="41"/>
       <c r="I11" s="12"/>
-      <c r="J11" s="41">
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41">
         <v>1</v>
       </c>
-      <c r="K11" s="41">
-        <v>150</v>
-      </c>
-      <c r="L11" s="41">
-        <f t="shared" si="5"/>
-        <v>150</v>
-      </c>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
+      <c r="N11" s="41">
+        <v>34000</v>
+      </c>
       <c r="O11" s="41">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="O11:O24" si="10">N11*M11</f>
+        <v>34000</v>
       </c>
       <c r="P11" s="12">
-        <f t="shared" si="4"/>
-        <v>150</v>
+        <f t="shared" ref="P11:P24" si="11">O11+L11</f>
+        <v>34000</v>
       </c>
       <c r="Q11" s="16">
-        <f t="shared" si="6"/>
-        <v>0.68181818181818177</v>
+        <f>P11/(SQRT(3)*380)</f>
+        <v>51.657655664334939</v>
       </c>
       <c r="R11" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2029,24 +2004,24 @@
         <v>1</v>
       </c>
       <c r="T11" s="41">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="U11" s="16">
-        <f>(T11*Maquinas!$H$12)*'Quadro de cargas'!V11</f>
-        <v>0.18483061749571181</v>
+        <f>(T11*Maquinas!H13)*'Quadro de cargas'!V11</f>
+        <v>2.7924374241192376</v>
       </c>
       <c r="V11" s="16">
         <f t="shared" si="2"/>
-        <v>0.6432246998284733</v>
+        <v>48.7336374191839</v>
       </c>
       <c r="W11" s="41">
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="X11" s="41">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="Y11" s="41" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2054,10 +2029,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="0"/>
@@ -2073,27 +2048,24 @@
       <c r="I12" s="12"/>
       <c r="J12" s="41"/>
       <c r="K12" s="41"/>
-      <c r="L12" s="41">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="L12" s="41"/>
       <c r="M12" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12" s="41">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="O12" s="41">
-        <f t="shared" si="3"/>
-        <v>2500</v>
+        <f t="shared" si="10"/>
+        <v>4000</v>
       </c>
       <c r="P12" s="12">
-        <f t="shared" si="4"/>
-        <v>2500</v>
+        <f t="shared" si="11"/>
+        <v>4000</v>
       </c>
       <c r="Q12" s="16">
-        <f>P12/(SQRT(3)*380)</f>
-        <v>3.798357034142275</v>
+        <f>P12/220</f>
+        <v>18.181818181818183</v>
       </c>
       <c r="R12" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2103,24 +2075,24 @@
         <v>1</v>
       </c>
       <c r="T12" s="41">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="U12" s="16">
-        <f>(T12*Maquinas!$H$12)*'Quadro de cargas'!V12</f>
-        <v>0.58838700472279393</v>
+        <f>(T12*Maquinas!H11)*'Quadro de cargas'!V12</f>
+        <v>2.5471698113207553</v>
       </c>
       <c r="V12" s="16">
         <f t="shared" si="2"/>
-        <v>3.5833556925870518</v>
+        <v>17.152658662092627</v>
       </c>
       <c r="W12" s="41">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="X12" s="41">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Y12" s="41" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2128,18 +2100,18 @@
         <v>10</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D13" s="16">
-        <f t="shared" si="0"/>
-        <v>257.64000000000004</v>
+        <f>7*7.4</f>
+        <v>51.800000000000004</v>
       </c>
       <c r="E13" s="16">
-        <f t="shared" si="1"/>
-        <v>68.2</v>
+        <f>7*2+2*7.4</f>
+        <v>28.8</v>
       </c>
       <c r="F13" s="41"/>
       <c r="G13" s="41"/>
@@ -2147,27 +2119,24 @@
       <c r="I13" s="12"/>
       <c r="J13" s="41"/>
       <c r="K13" s="41"/>
-      <c r="L13" s="41">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="L13" s="41"/>
       <c r="M13" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N13" s="41">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="O13" s="41">
-        <f t="shared" ref="O13:O15" si="7">N13*M13</f>
-        <v>2500</v>
+        <f t="shared" ref="O13:O14" si="12">N13*M13</f>
+        <v>6000</v>
       </c>
       <c r="P13" s="12">
-        <f t="shared" ref="P13:P16" si="8">O13+L13</f>
-        <v>2500</v>
+        <f t="shared" ref="P13:P14" si="13">O13+L13</f>
+        <v>6000</v>
       </c>
       <c r="Q13" s="16">
-        <f t="shared" ref="Q13:Q15" si="9">P13/(SQRT(3)*380)</f>
-        <v>3.798357034142275</v>
+        <f t="shared" ref="Q13:Q14" si="14">P13/220</f>
+        <v>27.272727272727273</v>
       </c>
       <c r="R13" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2177,24 +2146,24 @@
         <v>1</v>
       </c>
       <c r="T13" s="41">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="U13" s="16">
-        <f>(T13*Maquinas!$H$12)*'Quadro de cargas'!V13</f>
-        <v>0.58838700472279393</v>
+        <f>(T13*Maquinas!$H$11)*'Quadro de cargas'!V13</f>
+        <v>3.8207547169811327</v>
       </c>
       <c r="V13" s="16">
         <f t="shared" si="2"/>
-        <v>3.5833556925870518</v>
+        <v>25.728987993138936</v>
       </c>
       <c r="W13" s="41">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="X13" s="41">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="Y13" s="41" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2202,18 +2171,18 @@
         <v>11</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D14" s="16">
-        <f t="shared" si="0"/>
-        <v>257.64000000000004</v>
+        <f>7*7.4</f>
+        <v>51.800000000000004</v>
       </c>
       <c r="E14" s="16">
-        <f t="shared" si="1"/>
-        <v>68.2</v>
+        <f>7*2+2*7.4</f>
+        <v>28.8</v>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="41"/>
@@ -2221,27 +2190,24 @@
       <c r="I14" s="12"/>
       <c r="J14" s="41"/>
       <c r="K14" s="41"/>
-      <c r="L14" s="41">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="L14" s="41"/>
       <c r="M14" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N14" s="41">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="O14" s="41">
-        <f t="shared" si="7"/>
-        <v>2500</v>
+        <f t="shared" si="12"/>
+        <v>6000</v>
       </c>
       <c r="P14" s="12">
-        <f t="shared" si="8"/>
-        <v>2500</v>
+        <f t="shared" si="13"/>
+        <v>6000</v>
       </c>
       <c r="Q14" s="16">
-        <f t="shared" si="9"/>
-        <v>3.798357034142275</v>
+        <f t="shared" si="14"/>
+        <v>27.272727272727273</v>
       </c>
       <c r="R14" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2251,24 +2217,24 @@
         <v>1</v>
       </c>
       <c r="T14" s="41">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="U14" s="16">
-        <f>(T14*Maquinas!$H$12)*'Quadro de cargas'!V14</f>
-        <v>0.58838700472279393</v>
+        <f>(T14*Maquinas!$H$11)*'Quadro de cargas'!V14</f>
+        <v>3.8207547169811327</v>
       </c>
       <c r="V14" s="16">
         <f t="shared" si="2"/>
-        <v>3.5833556925870518</v>
+        <v>25.728987993138936</v>
       </c>
       <c r="W14" s="41">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="X14" s="41">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="Y14" s="41" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2276,18 +2242,18 @@
         <v>12</v>
       </c>
       <c r="B15" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>109</v>
-      </c>
       <c r="D15" s="16">
-        <f t="shared" si="0"/>
-        <v>257.64000000000004</v>
+        <f>7*7.4</f>
+        <v>51.800000000000004</v>
       </c>
       <c r="E15" s="16">
-        <f t="shared" si="1"/>
-        <v>68.2</v>
+        <f>7*2+2*7.4</f>
+        <v>28.8</v>
       </c>
       <c r="F15" s="41"/>
       <c r="G15" s="41"/>
@@ -2295,27 +2261,24 @@
       <c r="I15" s="12"/>
       <c r="J15" s="41"/>
       <c r="K15" s="41"/>
-      <c r="L15" s="41">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="L15" s="41"/>
       <c r="M15" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N15" s="41">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="O15" s="41">
-        <f t="shared" si="7"/>
-        <v>2500</v>
+        <f t="shared" si="10"/>
+        <v>6000</v>
       </c>
       <c r="P15" s="12">
-        <f t="shared" si="8"/>
-        <v>2500</v>
+        <f t="shared" si="11"/>
+        <v>6000</v>
       </c>
       <c r="Q15" s="16">
-        <f t="shared" si="9"/>
-        <v>3.798357034142275</v>
+        <f>P15/220</f>
+        <v>27.272727272727273</v>
       </c>
       <c r="R15" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2325,24 +2288,24 @@
         <v>1</v>
       </c>
       <c r="T15" s="41">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="U15" s="16">
-        <f>(T15*Maquinas!$H$12)*'Quadro de cargas'!V15</f>
-        <v>0.58838700472279393</v>
+        <f>(T15*Maquinas!H12)*'Quadro de cargas'!V15</f>
+        <v>6.3370497427101204</v>
       </c>
       <c r="V15" s="16">
         <f t="shared" si="2"/>
-        <v>3.5833556925870518</v>
+        <v>25.728987993138936</v>
       </c>
       <c r="W15" s="41">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="X15" s="41">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="Y15" s="41" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2350,18 +2313,18 @@
         <v>13</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D16" s="16">
-        <f t="shared" si="0"/>
-        <v>257.64000000000004</v>
+        <f t="shared" ref="D16:D19" si="15">11.26*4.5</f>
+        <v>50.67</v>
       </c>
       <c r="E16" s="16">
-        <f t="shared" si="1"/>
-        <v>68.2</v>
+        <f>11.26*2+2*4.5</f>
+        <v>31.52</v>
       </c>
       <c r="F16" s="41"/>
       <c r="G16" s="41"/>
@@ -2369,28 +2332,24 @@
       <c r="I16" s="12"/>
       <c r="J16" s="41"/>
       <c r="K16" s="41"/>
-      <c r="L16" s="41">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
+      <c r="L16" s="41"/>
       <c r="M16" s="41">
         <v>1</v>
       </c>
       <c r="N16" s="41">
-        <f>220*8</f>
-        <v>1760</v>
+        <v>2000</v>
       </c>
       <c r="O16" s="41">
-        <f>N16*M16</f>
-        <v>1760</v>
+        <f t="shared" si="10"/>
+        <v>2000</v>
       </c>
       <c r="P16" s="12">
-        <f t="shared" si="8"/>
-        <v>1760</v>
+        <f t="shared" si="11"/>
+        <v>2000</v>
       </c>
       <c r="Q16" s="16">
         <f>P16/220</f>
-        <v>8</v>
+        <v>9.0909090909090917</v>
       </c>
       <c r="R16" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2400,15 +2359,15 @@
         <v>1</v>
       </c>
       <c r="T16" s="41">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="U16" s="16">
-        <f>(T16*Maquinas!$H$12)*'Quadro de cargas'!V16</f>
-        <v>1.5490566037735849</v>
+        <f>(T16*Maquinas!$H$11)*'Quadro de cargas'!V16</f>
+        <v>0.42452830188679253</v>
       </c>
       <c r="V16" s="16">
-        <f>Q16/(R16*S16)</f>
-        <v>7.5471698113207539</v>
+        <f t="shared" si="2"/>
+        <v>8.5763293310463133</v>
       </c>
       <c r="W16" s="41">
         <v>2.5</v>
@@ -2425,18 +2384,18 @@
         <v>14</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D17" s="16">
-        <f t="shared" si="0"/>
-        <v>257.64000000000004</v>
+        <f t="shared" si="15"/>
+        <v>50.67</v>
       </c>
       <c r="E17" s="16">
-        <f t="shared" si="1"/>
-        <v>68.2</v>
+        <f t="shared" ref="E17:E20" si="16">11.26*2+2*4.5</f>
+        <v>31.52</v>
       </c>
       <c r="F17" s="41"/>
       <c r="G17" s="41"/>
@@ -2449,20 +2408,20 @@
         <v>1</v>
       </c>
       <c r="N17" s="41">
-        <f>220*8</f>
-        <v>1760</v>
+        <f>12*220</f>
+        <v>2640</v>
       </c>
       <c r="O17" s="41">
-        <f>N17*M17</f>
-        <v>1760</v>
+        <f t="shared" si="10"/>
+        <v>2640</v>
       </c>
       <c r="P17" s="12">
-        <f t="shared" ref="P17:P31" si="10">O17+L17</f>
-        <v>1760</v>
+        <f t="shared" si="11"/>
+        <v>2640</v>
       </c>
       <c r="Q17" s="16">
         <f>P17/220</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R17" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2472,15 +2431,15 @@
         <v>1</v>
       </c>
       <c r="T17" s="41">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="U17" s="16">
-        <f>(T17*Maquinas!$H$12)*'Quadro de cargas'!V17</f>
-        <v>1.8588679245283017</v>
+        <f>(T17*Maquinas!$H$11)*'Quadro de cargas'!V17</f>
+        <v>0.56037735849056602</v>
       </c>
       <c r="V17" s="16">
         <f t="shared" si="2"/>
-        <v>7.5471698113207539</v>
+        <v>11.320754716981131</v>
       </c>
       <c r="W17" s="41">
         <v>2.5</v>
@@ -2500,15 +2459,15 @@
         <v>99</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D18" s="16">
-        <f t="shared" si="0"/>
-        <v>257.64000000000004</v>
+        <f t="shared" si="15"/>
+        <v>50.67</v>
       </c>
       <c r="E18" s="16">
-        <f t="shared" si="1"/>
-        <v>68.2</v>
+        <f t="shared" si="16"/>
+        <v>31.52</v>
       </c>
       <c r="F18" s="41"/>
       <c r="G18" s="41"/>
@@ -2521,19 +2480,20 @@
         <v>1</v>
       </c>
       <c r="N18" s="41">
-        <v>34000</v>
+        <f t="shared" ref="N18:N19" si="17">12*220</f>
+        <v>2640</v>
       </c>
       <c r="O18" s="41">
-        <f t="shared" ref="O18:O31" si="11">N18*M18</f>
-        <v>34000</v>
+        <f t="shared" si="10"/>
+        <v>2640</v>
       </c>
       <c r="P18" s="12">
-        <f t="shared" si="10"/>
-        <v>34000</v>
+        <f t="shared" si="11"/>
+        <v>2640</v>
       </c>
       <c r="Q18" s="16">
-        <f>P18/(SQRT(3)*380)</f>
-        <v>51.657655664334939</v>
+        <f t="shared" ref="Q18:Q19" si="18">P18/220</f>
+        <v>12</v>
       </c>
       <c r="R18" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2543,24 +2503,24 @@
         <v>1</v>
       </c>
       <c r="T18" s="41">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="U18" s="16">
-        <f>(T18*Maquinas!H13)*'Quadro de cargas'!V18</f>
-        <v>2.7924374241192376</v>
+        <f>(T18*Maquinas!$H$11)*'Quadro de cargas'!V18</f>
+        <v>0.56037735849056602</v>
       </c>
       <c r="V18" s="16">
         <f t="shared" si="2"/>
-        <v>48.7336374191839</v>
+        <v>11.320754716981131</v>
       </c>
       <c r="W18" s="41">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="X18" s="41">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="Y18" s="41" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2568,18 +2528,18 @@
         <v>16</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D19" s="16">
-        <f t="shared" si="0"/>
-        <v>257.64000000000004</v>
+        <f t="shared" si="15"/>
+        <v>50.67</v>
       </c>
       <c r="E19" s="16">
-        <f t="shared" si="1"/>
-        <v>68.2</v>
+        <f t="shared" si="16"/>
+        <v>31.52</v>
       </c>
       <c r="F19" s="41"/>
       <c r="G19" s="41"/>
@@ -2589,22 +2549,23 @@
       <c r="K19" s="41"/>
       <c r="L19" s="41"/>
       <c r="M19" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N19" s="41">
-        <v>2000</v>
+        <f t="shared" si="17"/>
+        <v>2640</v>
       </c>
       <c r="O19" s="41">
+        <f t="shared" si="10"/>
+        <v>2640</v>
+      </c>
+      <c r="P19" s="12">
         <f t="shared" si="11"/>
-        <v>4000</v>
-      </c>
-      <c r="P19" s="12">
-        <f t="shared" si="10"/>
-        <v>4000</v>
+        <v>2640</v>
       </c>
       <c r="Q19" s="16">
-        <f>P19/220</f>
-        <v>18.181818181818183</v>
+        <f t="shared" si="18"/>
+        <v>12</v>
       </c>
       <c r="R19" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2614,24 +2575,24 @@
         <v>1</v>
       </c>
       <c r="T19" s="41">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="U19" s="16">
-        <f>(T19*Maquinas!H11)*'Quadro de cargas'!V19</f>
-        <v>2.5471698113207553</v>
+        <f>(T19*Maquinas!$H$11)*'Quadro de cargas'!V19</f>
+        <v>0.56037735849056602</v>
       </c>
       <c r="V19" s="16">
         <f t="shared" si="2"/>
-        <v>17.152658662092627</v>
+        <v>11.320754716981131</v>
       </c>
       <c r="W19" s="41">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="X19" s="41">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="Y19" s="41" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2639,43 +2600,47 @@
         <v>17</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D20" s="16">
-        <f>7*7.4</f>
-        <v>51.800000000000004</v>
+        <f>11.26*4.5</f>
+        <v>50.67</v>
       </c>
       <c r="E20" s="16">
-        <f>7*2+2*7.4</f>
-        <v>28.8</v>
-      </c>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
+        <f t="shared" si="16"/>
+        <v>31.52</v>
+      </c>
+      <c r="F20" s="41">
+        <v>6</v>
+      </c>
+      <c r="G20" s="41">
+        <f>D20*12/F20</f>
+        <v>101.33999999999999</v>
+      </c>
       <c r="H20" s="41"/>
-      <c r="I20" s="12"/>
+      <c r="I20" s="12">
+        <f>G20*F20</f>
+        <v>608.04</v>
+      </c>
       <c r="J20" s="41"/>
       <c r="K20" s="41"/>
       <c r="L20" s="41"/>
-      <c r="M20" s="41">
-        <v>3</v>
-      </c>
-      <c r="N20" s="41">
-        <v>2000</v>
-      </c>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
       <c r="O20" s="41">
-        <f t="shared" ref="O20:O21" si="12">N20*M20</f>
-        <v>6000</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="P20" s="12">
-        <f t="shared" ref="P20:P21" si="13">O20+L20</f>
-        <v>6000</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="Q20" s="16">
-        <f t="shared" ref="Q20:Q21" si="14">P20/220</f>
-        <v>27.272727272727273</v>
+        <f>I20/220</f>
+        <v>2.7638181818181815</v>
       </c>
       <c r="R20" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2685,24 +2650,24 @@
         <v>1</v>
       </c>
       <c r="T20" s="41">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="U20" s="16">
         <f>(T20*Maquinas!$H$11)*'Quadro de cargas'!V20</f>
-        <v>3.8207547169811327</v>
+        <v>0.12906509433962263</v>
       </c>
       <c r="V20" s="16">
         <f t="shared" si="2"/>
-        <v>25.728987993138936</v>
+        <v>2.6073756432246995</v>
       </c>
       <c r="W20" s="41">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="X20" s="41">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y20" s="41" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2710,43 +2675,47 @@
         <v>18</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D21" s="16">
-        <f>7*7.4</f>
-        <v>51.800000000000004</v>
+        <f t="shared" ref="D21" si="19">11.3*22.8</f>
+        <v>257.64000000000004</v>
       </c>
       <c r="E21" s="16">
-        <f>7*2+2*7.4</f>
-        <v>28.8</v>
-      </c>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
+        <f t="shared" ref="E21" si="20">11.3*2+22.8*2</f>
+        <v>68.2</v>
+      </c>
+      <c r="F21" s="41">
+        <v>18</v>
+      </c>
+      <c r="G21" s="41">
+        <f>D21*11/F21</f>
+        <v>157.44666666666669</v>
+      </c>
       <c r="H21" s="41"/>
-      <c r="I21" s="12"/>
+      <c r="I21" s="12">
+        <f t="shared" ref="I21:I23" si="21">G21*F21</f>
+        <v>2834.0400000000004</v>
+      </c>
       <c r="J21" s="41"/>
       <c r="K21" s="41"/>
       <c r="L21" s="41"/>
-      <c r="M21" s="41">
-        <v>3</v>
-      </c>
-      <c r="N21" s="41">
-        <v>2000</v>
-      </c>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
       <c r="O21" s="41">
-        <f t="shared" si="12"/>
-        <v>6000</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="P21" s="12">
-        <f t="shared" si="13"/>
-        <v>6000</v>
+        <f t="shared" si="11"/>
+        <v>0</v>
       </c>
       <c r="Q21" s="16">
-        <f t="shared" si="14"/>
-        <v>27.272727272727273</v>
+        <f t="shared" ref="Q21:Q22" si="22">I21/220</f>
+        <v>12.882000000000001</v>
       </c>
       <c r="R21" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2760,20 +2729,20 @@
       </c>
       <c r="U21" s="16">
         <f>(T21*Maquinas!$H$11)*'Quadro de cargas'!V21</f>
-        <v>3.8207547169811327</v>
+        <v>1.8046952830188683</v>
       </c>
       <c r="V21" s="16">
         <f t="shared" si="2"/>
-        <v>25.728987993138936</v>
+        <v>12.152830188679246</v>
       </c>
       <c r="W21" s="41">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="X21" s="41">
+        <v>16</v>
+      </c>
+      <c r="Y21" s="41" t="s">
         <v>32</v>
-      </c>
-      <c r="Y21" s="41" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2781,10 +2750,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D22" s="16">
         <f>7*7.4</f>
@@ -2794,30 +2763,34 @@
         <f>7*2+2*7.4</f>
         <v>28.8</v>
       </c>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
+      <c r="F22" s="41">
+        <v>4</v>
+      </c>
+      <c r="G22" s="41">
+        <f t="shared" ref="G22" si="23">D22*10/F22</f>
+        <v>129.5</v>
+      </c>
       <c r="H22" s="41"/>
-      <c r="I22" s="12"/>
+      <c r="I22" s="12">
+        <f t="shared" si="21"/>
+        <v>518</v>
+      </c>
       <c r="J22" s="41"/>
       <c r="K22" s="41"/>
       <c r="L22" s="41"/>
-      <c r="M22" s="41">
-        <v>3</v>
-      </c>
-      <c r="N22" s="41">
-        <v>2000</v>
-      </c>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
       <c r="O22" s="41">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="12">
         <f t="shared" si="11"/>
-        <v>6000</v>
-      </c>
-      <c r="P22" s="12">
-        <f t="shared" si="10"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="Q22" s="16">
-        <f>P22/220</f>
-        <v>27.272727272727273</v>
+        <f t="shared" si="22"/>
+        <v>2.3545454545454545</v>
       </c>
       <c r="R22" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2827,24 +2800,24 @@
         <v>1</v>
       </c>
       <c r="T22" s="41">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U22" s="16">
-        <f>(T22*Maquinas!H12)*'Quadro de cargas'!V22</f>
-        <v>6.3370497427101204</v>
+        <f>(T22*Maquinas!$H$11)*'Quadro de cargas'!V22</f>
+        <v>0.38483490566037737</v>
       </c>
       <c r="V22" s="16">
         <f t="shared" si="2"/>
-        <v>25.728987993138936</v>
+        <v>2.2212692967409948</v>
       </c>
       <c r="W22" s="41">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="X22" s="41">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="Y22" s="41" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2852,43 +2825,41 @@
         <v>20</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C23" s="41" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="D23" s="16">
-        <f t="shared" ref="D23:D26" si="15">11.26*4.5</f>
-        <v>50.67</v>
-      </c>
-      <c r="E23" s="16">
-        <f>11.26*2+2*4.5</f>
-        <v>31.52</v>
-      </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
+        <f>19*2.5+27.4*7.8</f>
+        <v>261.21999999999997</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="41">
+        <v>12</v>
+      </c>
+      <c r="G23" s="41">
+        <f>D23*8/F23</f>
+        <v>174.14666666666665</v>
+      </c>
       <c r="H23" s="41"/>
-      <c r="I23" s="12"/>
+      <c r="I23" s="12">
+        <f t="shared" si="21"/>
+        <v>2089.7599999999998</v>
+      </c>
       <c r="J23" s="41"/>
       <c r="K23" s="41"/>
       <c r="L23" s="41"/>
-      <c r="M23" s="41">
-        <v>1</v>
-      </c>
-      <c r="N23" s="41">
-        <v>2000</v>
-      </c>
-      <c r="O23" s="41">
-        <f t="shared" si="11"/>
-        <v>2000</v>
-      </c>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
       <c r="P23" s="12">
-        <f t="shared" si="10"/>
-        <v>2000</v>
+        <f t="shared" ref="P23" si="24">O23+L23</f>
+        <v>0</v>
       </c>
       <c r="Q23" s="16">
-        <f>P23/220</f>
-        <v>9.0909090909090917</v>
+        <f t="shared" ref="Q23" si="25">I23/220</f>
+        <v>9.4989090909090894</v>
       </c>
       <c r="R23" s="41">
         <f>Parâmetros!$B$2</f>
@@ -2898,15 +2869,12 @@
         <v>1</v>
       </c>
       <c r="T23" s="41">
-        <v>10</v>
-      </c>
-      <c r="U23" s="16">
-        <f>(T23*Maquinas!$H$11)*'Quadro de cargas'!V23</f>
-        <v>0.42452830188679253</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="U23" s="16"/>
       <c r="V23" s="16">
         <f t="shared" si="2"/>
-        <v>8.5763293310463133</v>
+        <v>8.9612349914236695</v>
       </c>
       <c r="W23" s="41">
         <v>2.5</v>
@@ -2915,7 +2883,7 @@
         <v>16</v>
       </c>
       <c r="Y23" s="41" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2926,585 +2894,277 @@
         <v>104</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D24" s="16">
-        <f t="shared" si="15"/>
-        <v>50.67</v>
+        <f>19*10+7.8</f>
+        <v>197.8</v>
       </c>
       <c r="E24" s="16">
-        <f t="shared" ref="E24:E27" si="16">11.26*2+2*4.5</f>
-        <v>31.52</v>
-      </c>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+        <f>19*2+2*10</f>
+        <v>58</v>
+      </c>
+      <c r="F24" s="41">
+        <v>1</v>
+      </c>
+      <c r="G24" s="41">
+        <f>D24*10</f>
+        <v>1978</v>
+      </c>
       <c r="H24" s="41"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41">
+      <c r="I24" s="12">
+        <f>G24</f>
+        <v>1978</v>
+      </c>
+      <c r="J24" s="41">
         <v>1</v>
       </c>
-      <c r="N24" s="41">
-        <f>12*220</f>
-        <v>2640</v>
-      </c>
+      <c r="K24" s="41">
+        <v>10000</v>
+      </c>
+      <c r="L24" s="41">
+        <v>8000</v>
+      </c>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
       <c r="O24" s="41">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="12">
         <f t="shared" si="11"/>
-        <v>2640</v>
-      </c>
-      <c r="P24" s="12">
-        <f t="shared" si="10"/>
-        <v>2640</v>
+        <v>8000</v>
       </c>
       <c r="Q24" s="16">
-        <f>P24/220</f>
-        <v>12</v>
+        <f>P24/(SQRT(3)*380)</f>
+        <v>12.15474250925528</v>
       </c>
       <c r="R24" s="41">
         <f>Parâmetros!$B$2</f>
         <v>1.06</v>
       </c>
       <c r="S24" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T24" s="41">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="U24" s="16">
         <f>(T24*Maquinas!$H$11)*'Quadro de cargas'!V24</f>
-        <v>0.56037735849056602</v>
+        <v>0.56760354170578908</v>
       </c>
       <c r="V24" s="16">
         <f t="shared" si="2"/>
-        <v>11.320754716981131</v>
+        <v>5.733369108139283</v>
       </c>
       <c r="W24" s="41">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="X24" s="41">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="Y24" s="41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40">
-        <v>22</v>
-      </c>
-      <c r="B25" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="16">
-        <f t="shared" si="15"/>
-        <v>50.67</v>
-      </c>
-      <c r="E25" s="16">
-        <f t="shared" si="16"/>
-        <v>31.52</v>
-      </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41">
-        <v>1</v>
-      </c>
-      <c r="N25" s="41">
-        <f t="shared" ref="N25:N26" si="17">12*220</f>
-        <v>2640</v>
-      </c>
-      <c r="O25" s="41">
-        <f t="shared" si="11"/>
-        <v>2640</v>
-      </c>
-      <c r="P25" s="12">
-        <f t="shared" si="10"/>
-        <v>2640</v>
-      </c>
-      <c r="Q25" s="16">
-        <f t="shared" ref="Q25:Q26" si="18">P25/220</f>
-        <v>12</v>
-      </c>
-      <c r="R25" s="41">
-        <f>Parâmetros!$B$2</f>
-        <v>1.06</v>
-      </c>
-      <c r="S25" s="41">
-        <v>1</v>
-      </c>
-      <c r="T25" s="41">
-        <v>10</v>
-      </c>
-      <c r="U25" s="16">
-        <f>(T25*Maquinas!$H$11)*'Quadro de cargas'!V25</f>
-        <v>0.56037735849056602</v>
-      </c>
-      <c r="V25" s="16">
-        <f t="shared" si="2"/>
-        <v>11.320754716981131</v>
-      </c>
-      <c r="W25" s="41">
-        <v>2.5</v>
-      </c>
-      <c r="X25" s="41">
-        <v>16</v>
-      </c>
-      <c r="Y25" s="41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="40">
-        <v>23</v>
-      </c>
-      <c r="B26" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="16">
-        <f t="shared" si="15"/>
-        <v>50.67</v>
-      </c>
-      <c r="E26" s="16">
-        <f t="shared" si="16"/>
-        <v>31.52</v>
-      </c>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="42"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+    </row>
+    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="40"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="44"/>
+      <c r="E26" s="41"/>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
-      <c r="I26" s="12"/>
+      <c r="I26" s="41"/>
       <c r="J26" s="41"/>
       <c r="K26" s="41"/>
       <c r="L26" s="41"/>
-      <c r="M26" s="41">
-        <v>1</v>
-      </c>
-      <c r="N26" s="41">
-        <f t="shared" si="17"/>
-        <v>2640</v>
-      </c>
-      <c r="O26" s="41">
-        <f t="shared" si="11"/>
-        <v>2640</v>
-      </c>
-      <c r="P26" s="12">
-        <f t="shared" si="10"/>
-        <v>2640</v>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="41">
+        <f>SUM(P4:P24)</f>
+        <v>142980</v>
       </c>
       <c r="Q26" s="16">
-        <f t="shared" si="18"/>
-        <v>12</v>
-      </c>
-      <c r="R26" s="41">
-        <f>Parâmetros!$B$2</f>
-        <v>1.06</v>
-      </c>
-      <c r="S26" s="41">
-        <v>1</v>
-      </c>
-      <c r="T26" s="41">
-        <v>10</v>
-      </c>
-      <c r="U26" s="16">
-        <f>(T26*Maquinas!$H$11)*'Quadro de cargas'!V26</f>
-        <v>0.56037735849056602</v>
-      </c>
+        <f>SUM(Q4:Q24)</f>
+        <v>353.61440833401667</v>
+      </c>
+      <c r="R26" s="16"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
       <c r="V26" s="16">
-        <f t="shared" si="2"/>
-        <v>11.320754716981131</v>
-      </c>
-      <c r="W26" s="41">
-        <v>2.5</v>
-      </c>
-      <c r="X26" s="41">
-        <v>16</v>
-      </c>
-      <c r="Y26" s="41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="40">
-        <v>24</v>
-      </c>
-      <c r="B27" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="D27" s="16">
-        <f>11.26*4.5</f>
-        <v>50.67</v>
-      </c>
-      <c r="E27" s="16">
-        <f t="shared" si="16"/>
-        <v>31.52</v>
-      </c>
-      <c r="F27" s="41">
-        <v>6</v>
-      </c>
-      <c r="G27" s="41">
-        <f>D27*12/F27</f>
-        <v>101.33999999999999</v>
-      </c>
-      <c r="H27" s="41"/>
-      <c r="I27" s="12">
-        <f>G27*F27</f>
-        <v>608.04</v>
-      </c>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="12">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="16">
-        <f>I27/220</f>
-        <v>2.7638181818181815</v>
-      </c>
-      <c r="R27" s="41">
-        <f>Parâmetros!$B$2</f>
-        <v>1.06</v>
-      </c>
-      <c r="S27" s="41">
-        <v>1</v>
-      </c>
-      <c r="T27" s="41">
-        <v>10</v>
-      </c>
-      <c r="U27" s="16">
-        <f>(T27*Maquinas!$H$11)*'Quadro de cargas'!V27</f>
-        <v>0.12906509433962263</v>
-      </c>
-      <c r="V27" s="16">
-        <f t="shared" si="2"/>
-        <v>2.6073756432246995</v>
-      </c>
-      <c r="W27" s="41">
-        <v>2.5</v>
-      </c>
-      <c r="X27" s="41">
-        <v>16</v>
-      </c>
-      <c r="Y27" s="41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="40">
-        <v>25</v>
-      </c>
-      <c r="B28" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="C28" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D28" s="16">
-        <f t="shared" ref="D28" si="19">11.3*22.8</f>
-        <v>257.64000000000004</v>
-      </c>
-      <c r="E28" s="16">
-        <f t="shared" ref="E28" si="20">11.3*2+22.8*2</f>
-        <v>68.2</v>
-      </c>
-      <c r="F28" s="41">
-        <v>18</v>
-      </c>
-      <c r="G28" s="41">
-        <f>D28*11/F28</f>
-        <v>157.44666666666669</v>
-      </c>
-      <c r="H28" s="41"/>
-      <c r="I28" s="12">
-        <f t="shared" ref="I28:I30" si="21">G28*F28</f>
-        <v>2834.0400000000004</v>
-      </c>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="12">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="16">
-        <f t="shared" ref="Q28:Q29" si="22">I28/220</f>
-        <v>12.882000000000001</v>
-      </c>
-      <c r="R28" s="41">
-        <f>Parâmetros!$B$2</f>
-        <v>1.06</v>
-      </c>
-      <c r="S28" s="41">
-        <v>1</v>
-      </c>
-      <c r="T28" s="41">
-        <v>30</v>
-      </c>
-      <c r="U28" s="16">
-        <f>(T28*Maquinas!$H$11)*'Quadro de cargas'!V28</f>
-        <v>1.8046952830188683</v>
-      </c>
-      <c r="V28" s="16">
-        <f t="shared" si="2"/>
-        <v>12.152830188679246</v>
-      </c>
-      <c r="W28" s="41">
-        <v>2.5</v>
-      </c>
-      <c r="X28" s="41">
-        <v>16</v>
-      </c>
-      <c r="Y28" s="41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="40">
-        <v>26</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="16">
-        <f>7*7.4</f>
-        <v>51.800000000000004</v>
-      </c>
-      <c r="E29" s="16">
-        <f>7*2+2*7.4</f>
-        <v>28.8</v>
-      </c>
-      <c r="F29" s="41">
-        <v>4</v>
-      </c>
-      <c r="G29" s="41">
-        <f t="shared" ref="G28:G30" si="23">D29*10/F29</f>
-        <v>129.5</v>
-      </c>
-      <c r="H29" s="41"/>
-      <c r="I29" s="12">
-        <f t="shared" si="21"/>
-        <v>518</v>
-      </c>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="12">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="16">
-        <f t="shared" si="22"/>
-        <v>2.3545454545454545</v>
-      </c>
-      <c r="R29" s="41">
-        <f>Parâmetros!$B$2</f>
-        <v>1.06</v>
-      </c>
-      <c r="S29" s="41">
-        <v>1</v>
-      </c>
-      <c r="T29" s="41">
-        <v>35</v>
-      </c>
-      <c r="U29" s="16">
-        <f>(T29*Maquinas!$H$11)*'Quadro de cargas'!V29</f>
-        <v>0.38483490566037737</v>
-      </c>
-      <c r="V29" s="16">
-        <f t="shared" si="2"/>
-        <v>2.2212692967409948</v>
-      </c>
-      <c r="W29" s="41">
-        <v>2.5</v>
-      </c>
-      <c r="X29" s="41">
-        <v>16</v>
-      </c>
-      <c r="Y29" s="41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="40">
-        <v>27</v>
-      </c>
-      <c r="B30" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="D30" s="16">
-        <f>19*2.5+27.4*7.8</f>
-        <v>261.21999999999997</v>
-      </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="41">
-        <v>12</v>
-      </c>
-      <c r="G30" s="41">
-        <f>D30*8/F30</f>
-        <v>174.14666666666665</v>
-      </c>
-      <c r="H30" s="41"/>
-      <c r="I30" s="12">
-        <f t="shared" si="21"/>
-        <v>2089.7599999999998</v>
-      </c>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="12">
-        <f t="shared" ref="P30" si="24">O30+L30</f>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="16">
-        <f t="shared" ref="Q30" si="25">I30/220</f>
-        <v>9.4989090909090894</v>
-      </c>
-      <c r="R30" s="41">
-        <f>Parâmetros!$B$2</f>
-        <v>1.06</v>
-      </c>
-      <c r="S30" s="41">
-        <v>1</v>
-      </c>
-      <c r="T30" s="41">
-        <v>35</v>
-      </c>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16">
-        <f t="shared" si="2"/>
-        <v>8.9612349914236695</v>
-      </c>
-      <c r="W30" s="41">
-        <v>2.5</v>
-      </c>
-      <c r="X30" s="41">
-        <v>16</v>
-      </c>
-      <c r="Y30" s="41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="40">
-        <v>28</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="16">
-        <f>19*10+7.8</f>
-        <v>197.8</v>
-      </c>
-      <c r="E31" s="16">
-        <f>19*2+2*10</f>
-        <v>58</v>
-      </c>
-      <c r="F31" s="41">
-        <v>1</v>
-      </c>
-      <c r="G31" s="41">
-        <f>D31*10</f>
-        <v>1978</v>
-      </c>
-      <c r="H31" s="41"/>
-      <c r="I31" s="12">
-        <f>G31</f>
-        <v>1978</v>
-      </c>
-      <c r="J31" s="41">
-        <v>1</v>
-      </c>
-      <c r="K31" s="41">
-        <v>10000</v>
-      </c>
-      <c r="L31" s="41">
-        <v>8000</v>
-      </c>
-      <c r="M31" s="41"/>
-      <c r="N31" s="41"/>
-      <c r="O31" s="41">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P31" s="12">
-        <f t="shared" si="10"/>
-        <v>8000</v>
-      </c>
-      <c r="Q31" s="16">
-        <f>P31/(SQRT(3)*380)</f>
-        <v>12.15474250925528</v>
-      </c>
-      <c r="R31" s="41">
-        <f>Parâmetros!$B$2</f>
-        <v>1.06</v>
-      </c>
-      <c r="S31" s="41">
-        <v>2</v>
-      </c>
-      <c r="T31" s="41">
-        <v>20</v>
-      </c>
-      <c r="U31" s="16">
-        <f>(T31*Maquinas!$H$11)*'Quadro de cargas'!V31</f>
-        <v>0.56760354170578908</v>
-      </c>
-      <c r="V31" s="16">
-        <f t="shared" si="2"/>
-        <v>5.733369108139283</v>
-      </c>
-      <c r="W31" s="41">
-        <v>2.5</v>
-      </c>
-      <c r="X31" s="41">
-        <v>16</v>
-      </c>
-      <c r="Y31" s="41" t="s">
-        <v>86</v>
-      </c>
+        <f>SUM(V4:V24)</f>
+        <v>327.86512932017837</v>
+      </c>
+      <c r="W26" s="46"/>
+      <c r="X26" s="41"/>
+      <c r="Y26" s="41"/>
+    </row>
+    <row r="27" spans="1:25" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="U27" s="43"/>
+      <c r="V27" s="41">
+        <f>V26*Parâmetros!B1</f>
+        <v>72130.328450439236</v>
+      </c>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
@@ -3527,248 +3187,49 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
-      <c r="V32" s="42"/>
+      <c r="V32" s="2"/>
       <c r="W32" s="2"/>
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="40"/>
-      <c r="B33" s="41"/>
-      <c r="C33" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="41"/>
-      <c r="N33" s="41"/>
-      <c r="O33" s="41"/>
-      <c r="P33" s="41">
-        <f>SUM(P4:P31)</f>
-        <v>212040</v>
-      </c>
-      <c r="Q33" s="16">
-        <f>SUM(Q4:Q31)</f>
-        <v>470.8262366762612</v>
-      </c>
-      <c r="R33" s="16"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="16"/>
-      <c r="U33" s="16"/>
-      <c r="V33" s="16">
-        <f>SUM(V4:V31)</f>
-        <v>438.44232586946572</v>
-      </c>
-      <c r="W33" s="46"/>
-      <c r="X33" s="41"/>
-      <c r="Y33" s="41"/>
-    </row>
-    <row r="34" spans="1:25" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="U34" s="43"/>
-      <c r="V34" s="41">
-        <f>V33*Parâmetros!B1</f>
-        <v>96457.311691282463</v>
-      </c>
-      <c r="W34" s="2"/>
-      <c r="X34" s="2"/>
-      <c r="Y34" s="2"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="2"/>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="2"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="2"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
-      <c r="W37" s="2"/>
-      <c r="X37" s="2"/>
-      <c r="Y37" s="2"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="2"/>
-      <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
-      <c r="W38" s="2"/>
-      <c r="X38" s="2"/>
-      <c r="Y38" s="2"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
-      <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
-      <c r="W39" s="2"/>
-      <c r="X39" s="2"/>
-      <c r="Y39" s="2"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
-      <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
-      <c r="W40" s="2"/>
-      <c r="X40" s="2"/>
-      <c r="Y40" s="2"/>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F1:I2"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="Y2:Y3"/>
     <mergeCell ref="U2:U3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="W2:W3"/>
-    <mergeCell ref="F1:I2"/>
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:P3"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:T3"/>
@@ -3810,7 +3271,7 @@
         <v>79</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>55</v>
@@ -3961,10 +3422,10 @@
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
       <c r="G10" s="34" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4177,15 +3638,15 @@
         <v>39</v>
       </c>
       <c r="B4" s="29">
-        <f>SUM('Quadro de cargas'!V4:V5)*Parâmetros!B1</f>
-        <v>37840.236113719264</v>
+        <f>SUM('Quadro de cargas'!V4:V4)*Parâmetros!B1</f>
+        <v>18920.118056859632</v>
       </c>
       <c r="C4" s="30">
         <v>1</v>
       </c>
       <c r="D4" s="29">
         <f>C4*B4</f>
-        <v>37840.236113719264</v>
+        <v>18920.118056859632</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4618,28 +4079,28 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F30" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G30" t="s">
         <v>24</v>
       </c>
       <c r="H30" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="I30" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
diagrama unifilar e quadro de cargas
</commit_message>
<xml_diff>
--- a/Quadro de cargas - Maquinas.xlsx
+++ b/Quadro de cargas - Maquinas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\Documents\Giovani\UCS\Instalações Elétricas (2)\UCS_Projeto_Instala-es_Industriais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA57FD6-F538-443F-A73E-754EABB66814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B5D09E-99F4-458E-A470-2FA1B5A40C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2475" windowWidth="20640" windowHeight="11760" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="606" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quadro de cargas" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="119">
   <si>
     <t>Cargas de Iluminação</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>T</t>
-  </si>
-  <si>
-    <t>Potência</t>
   </si>
   <si>
     <t>Demanda iluminação</t>
@@ -806,13 +803,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1278,9 +1275,9 @@
   </sheetPr>
   <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1308,21 +1305,21 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52" t="s">
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
@@ -1339,52 +1336,52 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="52" t="s">
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52" t="s">
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52" t="s">
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="50" t="s">
+      <c r="Q2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="50" t="s">
+      <c r="R2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="50" t="s">
+      <c r="S2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="50" t="s">
+      <c r="T2" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" s="50" t="s">
+      <c r="U2" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="V2" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="50" t="s">
+      <c r="W2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="50" t="s">
+      <c r="X2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="Y2" s="50" t="s">
+      <c r="Y2" s="52" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" s="9" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
@@ -1430,26 +1427,26 @@
       <c r="O3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="51"/>
-      <c r="U3" s="51"/>
-      <c r="V3" s="51"/>
-      <c r="W3" s="51"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
     </row>
     <row r="4" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40">
         <v>1</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="16">
         <f>11.3*22.8</f>
@@ -1508,7 +1505,7 @@
         <v>100</v>
       </c>
       <c r="Y4" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1516,10 +1513,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="16">
         <f t="shared" ref="D5:D12" si="0">11.3*22.8</f>
@@ -1579,7 +1576,7 @@
         <v>16</v>
       </c>
       <c r="Y5" s="41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1587,10 +1584,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="16">
         <f t="shared" si="0"/>
@@ -1661,10 +1658,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" s="16">
         <f t="shared" si="0"/>
@@ -1735,10 +1732,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" s="16">
         <f t="shared" si="0"/>
@@ -1801,7 +1798,7 @@
         <v>16</v>
       </c>
       <c r="Y8" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1809,10 +1806,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="16">
         <f t="shared" si="0"/>
@@ -1875,7 +1872,7 @@
         <v>16</v>
       </c>
       <c r="Y9" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1883,10 +1880,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="16">
         <f t="shared" si="0"/>
@@ -1958,10 +1955,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="0"/>
@@ -2021,7 +2018,7 @@
         <v>50</v>
       </c>
       <c r="Y11" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2029,10 +2026,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="0"/>
@@ -2089,7 +2086,7 @@
         <v>4</v>
       </c>
       <c r="X12" s="41">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="Y12" s="41" t="s">
         <v>32</v>
@@ -2100,10 +2097,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" s="16">
         <f>7*7.4</f>
@@ -2171,10 +2168,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="16">
         <f>7*7.4</f>
@@ -2242,10 +2239,10 @@
         <v>12</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15" s="16">
         <f>7*7.4</f>
@@ -2313,10 +2310,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="41" t="s">
         <v>95</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>96</v>
       </c>
       <c r="D16" s="16">
         <f t="shared" ref="D16:D19" si="15">11.26*4.5</f>
@@ -2384,10 +2381,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="15"/>
@@ -2456,10 +2453,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D18" s="16">
         <f t="shared" si="15"/>
@@ -2528,10 +2525,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" si="15"/>
@@ -2600,10 +2597,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="16">
         <f>11.26*4.5</f>
@@ -2675,10 +2672,10 @@
         <v>18</v>
       </c>
       <c r="B21" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="41" t="s">
         <v>101</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>102</v>
       </c>
       <c r="D21" s="16">
         <f t="shared" ref="D21" si="19">11.3*22.8</f>
@@ -2750,10 +2747,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D22" s="16">
         <f>7*7.4</f>
@@ -2825,10 +2822,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="41" t="s">
         <v>111</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>112</v>
       </c>
       <c r="D23" s="16">
         <f>19*2.5+27.4*7.8</f>
@@ -2891,10 +2888,10 @@
         <v>21</v>
       </c>
       <c r="B24" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="16">
         <f>19*10+7.8</f>
@@ -2964,7 +2961,7 @@
         <v>32</v>
       </c>
       <c r="Y24" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -3050,14 +3047,9 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
-      <c r="T27" s="43" t="s">
-        <v>33</v>
-      </c>
+      <c r="T27" s="43"/>
       <c r="U27" s="43"/>
-      <c r="V27" s="41">
-        <f>V26*Parâmetros!B1</f>
-        <v>72130.328450439236</v>
-      </c>
+      <c r="V27" s="41"/>
       <c r="W27" s="2"/>
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
@@ -3220,11 +3212,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="F1:I2"/>
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:P3"/>
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="Y2:Y3"/>
     <mergeCell ref="U2:U3"/>
@@ -3234,6 +3221,11 @@
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:T3"/>
     <mergeCell ref="V2:V3"/>
+    <mergeCell ref="F1:I2"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:P3"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.563194444444444" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="8" scale="74" fitToWidth="0" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3262,29 +3254,29 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>55</v>
       </c>
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="35">
         <f>1000/(SQRT(3)*380*1)</f>
@@ -3292,17 +3284,17 @@
       </c>
       <c r="D2" s="35"/>
       <c r="E2" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="35">
         <f>120/220</f>
@@ -3310,17 +3302,17 @@
       </c>
       <c r="D3" s="35"/>
       <c r="E3" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="35" t="s">
         <v>60</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>61</v>
       </c>
       <c r="C4" s="35">
         <f>2000/(SQRT(3)*380*1)</f>
@@ -3328,17 +3320,17 @@
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="35">
         <f>68000/(SQRT(3)*380*1)</f>
@@ -3349,17 +3341,17 @@
         <v>5.5400000000000002E-4</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>66</v>
-      </c>
-      <c r="B6" s="35" t="s">
-        <v>67</v>
       </c>
       <c r="C6" s="35">
         <f>34000/(SQRT(3)*380*1)</f>
@@ -3367,34 +3359,34 @@
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="35">
         <v>8</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="35">
         <f>1980/220</f>
@@ -3422,10 +3414,10 @@
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
       <c r="G10" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" t="s">
         <v>105</v>
-      </c>
-      <c r="H10" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3475,10 +3467,10 @@
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
@@ -3494,7 +3486,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="36">
         <v>300</v>
@@ -3511,7 +3503,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="36">
         <v>1000</v>
@@ -3521,7 +3513,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="36">
         <v>80</v>
@@ -3531,7 +3523,7 @@
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="36">
         <v>500</v>
@@ -3541,7 +3533,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="36">
         <v>100</v>
@@ -3551,7 +3543,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="36">
         <f>SUM(B15:B19)</f>
@@ -3592,18 +3584,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="29" t="e">
         <f>SUM('Quadro de cargas'!#REF!)*Parâmetros!B1</f>
@@ -3619,7 +3611,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="29" t="e">
         <f>(SUM('Quadro de cargas'!#REF!)-'Quadro de cargas'!#REF!)*Parâmetros!B1</f>
@@ -3635,7 +3627,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="29">
         <f>SUM('Quadro de cargas'!V4:V4)*Parâmetros!B1</f>
@@ -3651,7 +3643,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="29" t="e">
         <f>'Quadro de cargas'!#REF!*Parâmetros!B1</f>
@@ -3678,7 +3670,7 @@
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="26"/>
       <c r="C8" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="29" t="e">
         <f>SUM(D2:D6)</f>
@@ -3687,7 +3679,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="32" t="e">
         <f>D8/(Parâmetros!B3*SQRT(3))</f>
@@ -3696,15 +3688,15 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="32">
         <v>5.0999999999999996</v>
@@ -3712,7 +3704,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="32">
         <v>4</v>
@@ -3720,7 +3712,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="32">
         <f>3.1415*(D12/2)^2*D13</f>
@@ -3729,7 +3721,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="32">
         <v>1</v>
@@ -3737,7 +3729,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="32">
         <f>3.1415*((D16*25.4)/2)^2</f>
@@ -3746,7 +3738,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="33">
         <f>D14/D17</f>
@@ -4047,7 +4039,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>380</v>
@@ -4062,8 +4054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B241DD-D43C-40E0-9FBA-E2F87E7EF9B7}">
   <dimension ref="B25:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4079,28 +4071,28 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="s">
         <v>113</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>114</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" t="s">
         <v>115</v>
-      </c>
-      <c r="E30" t="s">
-        <v>117</v>
-      </c>
-      <c r="F30" t="s">
-        <v>116</v>
       </c>
       <c r="G30" t="s">
         <v>24</v>
       </c>
       <c r="H30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I30" t="s">
         <v>118</v>
-      </c>
-      <c r="I30" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>